<commit_message>
Réorganisation des tests progdyn
quelques données en plus dans excel
</commit_message>
<xml_diff>
--- a/tp2/exemple/src/result.xlsx
+++ b/tp2/exemple/src/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\01.Travaux.Poly\09.A2018\INF4705.algo\swagnalyse\tp2\exemple\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9C6463BF-2461-4A3C-B138-131644CA880A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{A9C5CD35-20B5-409B-9B0D-ECB82215439E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="78" yWindow="462" windowWidth="25440" windowHeight="14502" xr2:uid="{5E1C5933-FED9-854C-841B-467E1B961C4A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="278">
   <si>
     <t>glouton</t>
   </si>
@@ -841,6 +841,24 @@
   </si>
   <si>
     <t>recuit</t>
+  </si>
+  <si>
+    <t>progdyn1</t>
+  </si>
+  <si>
+    <t>progdyn2</t>
+  </si>
+  <si>
+    <t>0.953125</t>
+  </si>
+  <si>
+    <t>1.1875</t>
+  </si>
+  <si>
+    <t>1.046875</t>
+  </si>
+  <si>
+    <t>1.359375</t>
   </si>
 </sst>
 </file>
@@ -1201,10 +1219,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D3A866-B3F1-5D4F-A126-3B73E31B27BE}">
-  <dimension ref="A1:P270"/>
+  <dimension ref="A1:AC270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F40" workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="S8" sqref="S8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
@@ -1213,7 +1231,7 @@
     <col min="5" max="5" width="11.6484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="17.7">
+    <row r="1" spans="1:29" ht="17.7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1249,8 +1267,36 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="17.7">
+      <c r="R1" t="s">
+        <v>272</v>
+      </c>
+      <c r="S1">
+        <v>1999.09375</v>
+      </c>
+      <c r="T1">
+        <v>4059</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>273</v>
+      </c>
+      <c r="Z1">
+        <v>475.75</v>
+      </c>
+      <c r="AA1">
+        <v>4059</v>
+      </c>
+      <c r="AB1">
+        <v>4000</v>
+      </c>
+      <c r="AC1">
+        <f>AVERAGE(Z1:Z10)</f>
+        <v>878.21406249999995</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" ht="17.7">
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1266,8 +1312,23 @@
       <c r="N2">
         <v>3932</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" ht="17.7">
+      <c r="S2">
+        <v>2299.53125</v>
+      </c>
+      <c r="T2">
+        <v>4004</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z2">
+        <v>968.71875</v>
+      </c>
+      <c r="AA2">
+        <v>4004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" ht="17.7">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1283,8 +1344,23 @@
       <c r="N3">
         <v>3819</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" ht="17.7">
+      <c r="S3">
+        <v>2013.078125</v>
+      </c>
+      <c r="T3">
+        <v>4017</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z3">
+        <v>760.421875</v>
+      </c>
+      <c r="AA3">
+        <v>4017</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" ht="17.7">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -1300,8 +1376,23 @@
       <c r="N4">
         <v>3951</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" ht="17.7">
+      <c r="S4">
+        <v>2217.4375</v>
+      </c>
+      <c r="T4">
+        <v>4064</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z4">
+        <v>2098.5625</v>
+      </c>
+      <c r="AA4">
+        <v>4064</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" ht="17.7">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1317,8 +1408,23 @@
       <c r="N5">
         <v>3795</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" ht="17.7">
+      <c r="S5">
+        <v>2130.359375</v>
+      </c>
+      <c r="T5">
+        <v>4022</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z5">
+        <v>716.734375</v>
+      </c>
+      <c r="AA5">
+        <v>4022</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" ht="17.7">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1334,8 +1440,23 @@
       <c r="N6">
         <v>4090</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" ht="17.7">
+      <c r="S6">
+        <v>2318.5625</v>
+      </c>
+      <c r="T6">
+        <v>4190</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z6">
+        <v>773.609375</v>
+      </c>
+      <c r="AA6">
+        <v>4190</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" ht="17.7">
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1351,8 +1472,17 @@
       <c r="N7">
         <v>4050</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" ht="17.7">
+      <c r="V7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z7">
+        <v>842.25</v>
+      </c>
+      <c r="AA7">
+        <v>4188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" ht="17.7">
       <c r="B8" s="1" t="s">
         <v>8</v>
       </c>
@@ -1368,8 +1498,17 @@
       <c r="N8">
         <v>3878</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" ht="17.7">
+      <c r="V8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z8">
+        <v>358.640625</v>
+      </c>
+      <c r="AA8">
+        <v>4093</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" ht="17.7">
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
@@ -1385,8 +1524,17 @@
       <c r="N9">
         <v>3948</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" ht="17.7">
+      <c r="V9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z9">
+        <v>718.5</v>
+      </c>
+      <c r="AA9">
+        <v>4028</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" ht="17.7">
       <c r="B10" s="1" t="s">
         <v>10</v>
       </c>
@@ -1402,8 +1550,17 @@
       <c r="N10">
         <v>3879</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" ht="17.7">
+      <c r="V10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z10">
+        <v>1068.953125</v>
+      </c>
+      <c r="AA10">
+        <v>4005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="17.7">
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1417,7 +1574,7 @@
         <v>400</v>
       </c>
       <c r="H11">
-        <f t="shared" ref="H2:H65" si="0">AVERAGE(E11:E20)</f>
+        <f t="shared" ref="H11:H61" si="0">AVERAGE(E11:E20)</f>
         <v>1.0101795196533188E-4</v>
       </c>
       <c r="M11">
@@ -1433,8 +1590,30 @@
         <f>AVERAGE(M11:M20)</f>
         <v>1.6970634460449169E-4</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" ht="17.7">
+      <c r="S11" t="s">
+        <v>274</v>
+      </c>
+      <c r="T11">
+        <v>403</v>
+      </c>
+      <c r="V11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z11">
+        <v>2.40625</v>
+      </c>
+      <c r="AA11">
+        <v>402</v>
+      </c>
+      <c r="AB11">
+        <v>400</v>
+      </c>
+      <c r="AC11">
+        <f>AVERAGE(Z11:Z20)</f>
+        <v>3.0328124999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" ht="17.7">
       <c r="B12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1450,8 +1629,23 @@
       <c r="N12">
         <v>391</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" ht="17.7">
+      <c r="S12" t="s">
+        <v>275</v>
+      </c>
+      <c r="T12">
+        <v>438</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z12">
+        <v>3.125</v>
+      </c>
+      <c r="AA12">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" ht="17.7">
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
@@ -1467,8 +1661,23 @@
       <c r="N13">
         <v>382</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" ht="17.7">
+      <c r="S13" t="s">
+        <v>276</v>
+      </c>
+      <c r="T13">
+        <v>423</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z13">
+        <v>2.734375</v>
+      </c>
+      <c r="AA13">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" ht="17.7">
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
@@ -1484,8 +1693,23 @@
       <c r="N14">
         <v>404</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" ht="17.7">
+      <c r="S14" t="s">
+        <v>276</v>
+      </c>
+      <c r="T14">
+        <v>417</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z14">
+        <v>3.515625</v>
+      </c>
+      <c r="AA14">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" ht="17.7">
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
@@ -1501,8 +1725,23 @@
       <c r="N15">
         <v>397</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" ht="17.7">
+      <c r="S15" t="s">
+        <v>277</v>
+      </c>
+      <c r="T15">
+        <v>458</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z15">
+        <v>2.53125</v>
+      </c>
+      <c r="AA15">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" ht="17.7">
       <c r="B16" s="1" t="s">
         <v>16</v>
       </c>
@@ -1518,8 +1757,17 @@
       <c r="N16">
         <v>452</v>
       </c>
-    </row>
-    <row r="17" spans="2:16" ht="17.7">
+      <c r="V16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z16">
+        <v>4.109375</v>
+      </c>
+      <c r="AA16">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="17" spans="2:29" ht="17.7">
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
@@ -1535,8 +1783,17 @@
       <c r="N17">
         <v>399</v>
       </c>
-    </row>
-    <row r="18" spans="2:16" ht="17.7">
+      <c r="V17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z17">
+        <v>2.71875</v>
+      </c>
+      <c r="AA17">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="18" spans="2:29" ht="17.7">
       <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
@@ -1552,8 +1809,17 @@
       <c r="N18">
         <v>425</v>
       </c>
-    </row>
-    <row r="19" spans="2:16" ht="17.7">
+      <c r="V18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z18">
+        <v>2.484375</v>
+      </c>
+      <c r="AA18">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="19" spans="2:29" ht="17.7">
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
@@ -1569,8 +1835,17 @@
       <c r="N19">
         <v>401</v>
       </c>
-    </row>
-    <row r="20" spans="2:16" ht="17.7">
+      <c r="V19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z19">
+        <v>3.078125</v>
+      </c>
+      <c r="AA19">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="20" spans="2:29" ht="17.7">
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
@@ -1586,8 +1861,17 @@
       <c r="N20">
         <v>369</v>
       </c>
-    </row>
-    <row r="21" spans="2:16" ht="17.7">
+      <c r="V20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z20">
+        <v>3.625</v>
+      </c>
+      <c r="AA20">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="21" spans="2:29" ht="17.7">
       <c r="B21" s="1" t="s">
         <v>21</v>
       </c>
@@ -1617,8 +1901,24 @@
         <f>AVERAGE(M21:M30)</f>
         <v>2.3531913757324181E-4</v>
       </c>
-    </row>
-    <row r="22" spans="2:16" ht="17.7">
+      <c r="V21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z21">
+        <v>95.796875</v>
+      </c>
+      <c r="AA21">
+        <v>2050</v>
+      </c>
+      <c r="AB21">
+        <v>2000</v>
+      </c>
+      <c r="AC21">
+        <f>AVERAGE(Z21:Z30)</f>
+        <v>145.95156249999999</v>
+      </c>
+    </row>
+    <row r="22" spans="2:29" ht="17.7">
       <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
@@ -1634,8 +1934,17 @@
       <c r="N22">
         <v>2029</v>
       </c>
-    </row>
-    <row r="23" spans="2:16" ht="17.7">
+      <c r="V22" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z22">
+        <v>298.5625</v>
+      </c>
+      <c r="AA22">
+        <v>2031</v>
+      </c>
+    </row>
+    <row r="23" spans="2:29" ht="17.7">
       <c r="B23" s="1" t="s">
         <v>23</v>
       </c>
@@ -1651,8 +1960,17 @@
       <c r="N23">
         <v>1927</v>
       </c>
-    </row>
-    <row r="24" spans="2:16" ht="17.7">
+      <c r="V23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z23">
+        <v>94.234375</v>
+      </c>
+      <c r="AA23">
+        <v>2044</v>
+      </c>
+    </row>
+    <row r="24" spans="2:29" ht="17.7">
       <c r="B24" s="1" t="s">
         <v>24</v>
       </c>
@@ -1668,8 +1986,17 @@
       <c r="N24">
         <v>1991</v>
       </c>
-    </row>
-    <row r="25" spans="2:16" ht="17.7">
+      <c r="V24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z24">
+        <v>125.953125</v>
+      </c>
+      <c r="AA24">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="25" spans="2:29" ht="17.7">
       <c r="B25" s="1" t="s">
         <v>25</v>
       </c>
@@ -1685,8 +2012,17 @@
       <c r="N25">
         <v>1951</v>
       </c>
-    </row>
-    <row r="26" spans="2:16" ht="17.7">
+      <c r="V25" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z25">
+        <v>275.203125</v>
+      </c>
+      <c r="AA25">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="26" spans="2:29" ht="17.7">
       <c r="B26" s="1" t="s">
         <v>26</v>
       </c>
@@ -1702,8 +2038,17 @@
       <c r="N26">
         <v>1988</v>
       </c>
-    </row>
-    <row r="27" spans="2:16" ht="17.7">
+      <c r="V26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z26">
+        <v>156.59375</v>
+      </c>
+      <c r="AA26">
+        <v>2091</v>
+      </c>
+    </row>
+    <row r="27" spans="2:29" ht="17.7">
       <c r="B27" s="1" t="s">
         <v>27</v>
       </c>
@@ -1719,8 +2064,17 @@
       <c r="N27">
         <v>2056</v>
       </c>
-    </row>
-    <row r="28" spans="2:16" ht="17.7">
+      <c r="V27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z27">
+        <v>70.265625</v>
+      </c>
+      <c r="AA27">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="28" spans="2:29" ht="17.7">
       <c r="B28" s="1" t="s">
         <v>28</v>
       </c>
@@ -1736,8 +2090,17 @@
       <c r="N28">
         <v>1961</v>
       </c>
-    </row>
-    <row r="29" spans="2:16" ht="17.7">
+      <c r="V28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="Z28">
+        <v>128.453125</v>
+      </c>
+      <c r="AA28">
+        <v>2049</v>
+      </c>
+    </row>
+    <row r="29" spans="2:29" ht="17.7">
       <c r="B29" s="1" t="s">
         <v>29</v>
       </c>
@@ -1753,8 +2116,17 @@
       <c r="N29">
         <v>2010</v>
       </c>
-    </row>
-    <row r="30" spans="2:16" ht="17.7">
+      <c r="V29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z29">
+        <v>69.328125</v>
+      </c>
+      <c r="AA29">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="30" spans="2:29" ht="17.7">
       <c r="B30" s="1" t="s">
         <v>30</v>
       </c>
@@ -1770,8 +2142,17 @@
       <c r="N30">
         <v>1989</v>
       </c>
-    </row>
-    <row r="31" spans="2:16" ht="17.7">
+      <c r="V30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z30">
+        <v>145.125</v>
+      </c>
+      <c r="AA30">
+        <v>2069</v>
+      </c>
+    </row>
+    <row r="31" spans="2:29" ht="17.7">
       <c r="B31" s="2" t="s">
         <v>31</v>
       </c>
@@ -1801,8 +2182,24 @@
         <f>AVERAGE(M31:M40)</f>
         <v>1.0411739349365206E-4</v>
       </c>
-    </row>
-    <row r="32" spans="2:16" ht="17.7">
+      <c r="V31" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z31">
+        <v>0</v>
+      </c>
+      <c r="AA31">
+        <v>11</v>
+      </c>
+      <c r="AB31">
+        <v>10</v>
+      </c>
+      <c r="AC31">
+        <f>AVERAGE(Z31:Z40)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:29" ht="17.7">
       <c r="B32" s="2" t="s">
         <v>32</v>
       </c>
@@ -1818,8 +2215,17 @@
       <c r="N32">
         <v>11</v>
       </c>
-    </row>
-    <row r="33" spans="2:16" ht="17.7">
+      <c r="V32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z32">
+        <v>0</v>
+      </c>
+      <c r="AA32">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="2:29" ht="17.7">
       <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
@@ -1835,8 +2241,17 @@
       <c r="N33">
         <v>11</v>
       </c>
-    </row>
-    <row r="34" spans="2:16" ht="17.7">
+      <c r="V33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="2:29" ht="17.7">
       <c r="B34" s="2" t="s">
         <v>34</v>
       </c>
@@ -1852,8 +2267,17 @@
       <c r="N34">
         <v>9</v>
       </c>
-    </row>
-    <row r="35" spans="2:16" ht="17.7">
+      <c r="V34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z34">
+        <v>0</v>
+      </c>
+      <c r="AA34">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="2:29" ht="17.7">
       <c r="B35" s="2" t="s">
         <v>35</v>
       </c>
@@ -1869,8 +2293,17 @@
       <c r="N35">
         <v>10</v>
       </c>
-    </row>
-    <row r="36" spans="2:16" ht="17.7">
+      <c r="V35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Z35">
+        <v>0</v>
+      </c>
+      <c r="AA35">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="2:29" ht="17.7">
       <c r="B36" s="2" t="s">
         <v>36</v>
       </c>
@@ -1886,8 +2319,17 @@
       <c r="N36">
         <v>9</v>
       </c>
-    </row>
-    <row r="37" spans="2:16" ht="17.7">
+      <c r="V36" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Z36">
+        <v>0</v>
+      </c>
+      <c r="AA36">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="2:29" ht="17.7">
       <c r="B37" s="2" t="s">
         <v>37</v>
       </c>
@@ -1903,8 +2345,17 @@
       <c r="N37">
         <v>11</v>
       </c>
-    </row>
-    <row r="38" spans="2:16" ht="17.7">
+      <c r="V37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z37">
+        <v>0</v>
+      </c>
+      <c r="AA37">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="38" spans="2:29" ht="17.7">
       <c r="B38" s="2" t="s">
         <v>38</v>
       </c>
@@ -1920,8 +2371,17 @@
       <c r="N38">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="2:16" ht="17.7">
+      <c r="V38" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z38">
+        <v>0</v>
+      </c>
+      <c r="AA38">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="2:29" ht="17.7">
       <c r="B39" s="2" t="s">
         <v>39</v>
       </c>
@@ -1937,8 +2397,17 @@
       <c r="N39">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="2:16" ht="17.7">
+      <c r="V39" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z39">
+        <v>0</v>
+      </c>
+      <c r="AA39">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="40" spans="2:29" ht="17.7">
       <c r="B40" s="2" t="s">
         <v>40</v>
       </c>
@@ -1954,8 +2423,17 @@
       <c r="N40">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="2:16" ht="17.7">
+      <c r="V40" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z40">
+        <v>0</v>
+      </c>
+      <c r="AA40">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="41" spans="2:29" ht="17.7">
       <c r="B41" s="2" t="s">
         <v>41</v>
       </c>
@@ -1985,8 +2463,25 @@
         <f>AVERAGE(M41:M50)</f>
         <v>9.93728637695309E-5</v>
       </c>
-    </row>
-    <row r="42" spans="2:16" ht="17.7">
+      <c r="Q41" s="3"/>
+      <c r="V41" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z41">
+        <v>9.375E-2</v>
+      </c>
+      <c r="AA41">
+        <v>100</v>
+      </c>
+      <c r="AB41">
+        <v>100</v>
+      </c>
+      <c r="AC41" s="3">
+        <f>AVERAGE(Z41:Z50)</f>
+        <v>9.375E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="2:29" ht="17.7">
       <c r="B42" s="2" t="s">
         <v>42</v>
       </c>
@@ -2002,8 +2497,17 @@
       <c r="N42">
         <v>96</v>
       </c>
-    </row>
-    <row r="43" spans="2:16" ht="17.7">
+      <c r="V42" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Z42">
+        <v>0.109375</v>
+      </c>
+      <c r="AA42">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="2:29" ht="17.7">
       <c r="B43" s="2" t="s">
         <v>43</v>
       </c>
@@ -2019,8 +2523,17 @@
       <c r="N43">
         <v>44</v>
       </c>
-    </row>
-    <row r="44" spans="2:16" ht="17.7">
+      <c r="V43" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z43">
+        <v>7.8125E-2</v>
+      </c>
+      <c r="AA43">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="2:29" ht="17.7">
       <c r="B44" s="2" t="s">
         <v>44</v>
       </c>
@@ -2036,8 +2549,17 @@
       <c r="N44">
         <v>15</v>
       </c>
-    </row>
-    <row r="45" spans="2:16" ht="17.7">
+      <c r="V44" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z44">
+        <v>0.125</v>
+      </c>
+      <c r="AA44">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="2:29" ht="17.7">
       <c r="B45" s="2" t="s">
         <v>45</v>
       </c>
@@ -2053,8 +2575,17 @@
       <c r="N45">
         <v>76</v>
       </c>
-    </row>
-    <row r="46" spans="2:16" ht="17.7">
+      <c r="V45" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z45">
+        <v>0.125</v>
+      </c>
+      <c r="AA45">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="2:29" ht="17.7">
       <c r="B46" s="2" t="s">
         <v>46</v>
       </c>
@@ -2070,8 +2601,17 @@
       <c r="N46">
         <v>85</v>
       </c>
-    </row>
-    <row r="47" spans="2:16" ht="17.7">
+      <c r="V46" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z46">
+        <v>6.25E-2</v>
+      </c>
+      <c r="AA46">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="2:29" ht="17.7">
       <c r="B47" s="2" t="s">
         <v>47</v>
       </c>
@@ -2087,8 +2627,17 @@
       <c r="N47">
         <v>98</v>
       </c>
-    </row>
-    <row r="48" spans="2:16" ht="17.7">
+      <c r="V47" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z47">
+        <v>9.375E-2</v>
+      </c>
+      <c r="AA47">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="2:29" ht="17.7">
       <c r="B48" s="2" t="s">
         <v>48</v>
       </c>
@@ -2104,8 +2653,17 @@
       <c r="N48">
         <v>60</v>
       </c>
-    </row>
-    <row r="49" spans="2:16" ht="17.7">
+      <c r="V48" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z48">
+        <v>7.8125E-2</v>
+      </c>
+      <c r="AA48">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="2:29" ht="17.7">
       <c r="B49" s="2" t="s">
         <v>49</v>
       </c>
@@ -2121,8 +2679,17 @@
       <c r="N49">
         <v>60</v>
       </c>
-    </row>
-    <row r="50" spans="2:16" ht="17.7">
+      <c r="V49" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="Z49">
+        <v>7.8125E-2</v>
+      </c>
+      <c r="AA49">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="2:29" ht="17.7">
       <c r="B50" s="2" t="s">
         <v>50</v>
       </c>
@@ -2138,8 +2705,17 @@
       <c r="N50">
         <v>98</v>
       </c>
-    </row>
-    <row r="51" spans="2:16" ht="17.7">
+      <c r="V50" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z50">
+        <v>9.375E-2</v>
+      </c>
+      <c r="AA50">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="2:29" ht="17.7">
       <c r="B51" s="2" t="s">
         <v>51</v>
       </c>
@@ -2169,8 +2745,24 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="52" spans="2:16" ht="17.7">
+      <c r="V51" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z51">
+        <v>11.59375</v>
+      </c>
+      <c r="AA51">
+        <v>939</v>
+      </c>
+      <c r="AB51">
+        <v>1000</v>
+      </c>
+      <c r="AC51">
+        <f>AVERAGE(Z1:Z10)</f>
+        <v>878.21406249999995</v>
+      </c>
+    </row>
+    <row r="52" spans="2:29" ht="17.7">
       <c r="B52" s="2" t="s">
         <v>52</v>
       </c>
@@ -2186,8 +2778,17 @@
       <c r="N52">
         <v>658</v>
       </c>
-    </row>
-    <row r="53" spans="2:16" ht="17.7">
+      <c r="V52" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z52">
+        <v>10.515625</v>
+      </c>
+      <c r="AA52">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="53" spans="2:29" ht="17.7">
       <c r="B53" s="2" t="s">
         <v>53</v>
       </c>
@@ -2203,8 +2804,17 @@
       <c r="N53">
         <v>450</v>
       </c>
-    </row>
-    <row r="54" spans="2:16" ht="17.7">
+      <c r="V53" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z53">
+        <v>17.34375</v>
+      </c>
+      <c r="AA53">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="54" spans="2:29" ht="17.7">
       <c r="B54" s="2" t="s">
         <v>54</v>
       </c>
@@ -2220,8 +2830,17 @@
       <c r="N54">
         <v>783</v>
       </c>
-    </row>
-    <row r="55" spans="2:16" ht="17.7">
+      <c r="V54" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z54">
+        <v>12.796875</v>
+      </c>
+      <c r="AA54">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="55" spans="2:29" ht="17.7">
       <c r="B55" s="2" t="s">
         <v>55</v>
       </c>
@@ -2237,8 +2856,17 @@
       <c r="N55">
         <v>580</v>
       </c>
-    </row>
-    <row r="56" spans="2:16" ht="17.7">
+      <c r="V55" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z55">
+        <v>13.109375</v>
+      </c>
+      <c r="AA55">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="56" spans="2:29" ht="17.7">
       <c r="B56" s="2" t="s">
         <v>56</v>
       </c>
@@ -2254,8 +2882,17 @@
       <c r="N56">
         <v>914</v>
       </c>
-    </row>
-    <row r="57" spans="2:16" ht="17.7">
+      <c r="V56" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z56">
+        <v>12.796875</v>
+      </c>
+      <c r="AA56">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="57" spans="2:29" ht="17.7">
       <c r="B57" s="2" t="s">
         <v>57</v>
       </c>
@@ -2271,8 +2908,17 @@
       <c r="N57">
         <v>182</v>
       </c>
-    </row>
-    <row r="58" spans="2:16" ht="17.7">
+      <c r="V57" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z57">
+        <v>11.59375</v>
+      </c>
+      <c r="AA57">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="58" spans="2:29" ht="17.7">
       <c r="B58" s="2" t="s">
         <v>58</v>
       </c>
@@ -2288,8 +2934,17 @@
       <c r="N58">
         <v>963</v>
       </c>
-    </row>
-    <row r="59" spans="2:16" ht="17.7">
+      <c r="V58" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="Z58">
+        <v>18.90625</v>
+      </c>
+      <c r="AA58">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="59" spans="2:29" ht="17.7">
       <c r="B59" s="2" t="s">
         <v>59</v>
       </c>
@@ -2305,8 +2960,17 @@
       <c r="N59">
         <v>889</v>
       </c>
-    </row>
-    <row r="60" spans="2:16" ht="17.7">
+      <c r="V59" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z59">
+        <v>14.859375</v>
+      </c>
+      <c r="AA59">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="60" spans="2:29" ht="17.7">
       <c r="B60" s="2" t="s">
         <v>60</v>
       </c>
@@ -2322,8 +2986,17 @@
       <c r="N60">
         <v>814</v>
       </c>
-    </row>
-    <row r="61" spans="2:16" ht="17.7">
+      <c r="V60" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z60">
+        <v>20.046875</v>
+      </c>
+      <c r="AA60">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="61" spans="2:29" ht="17.7">
       <c r="B61" s="2" t="s">
         <v>61</v>
       </c>
@@ -2353,8 +3026,24 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="62" spans="2:16" ht="17.7">
+      <c r="V61" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z61">
+        <v>0</v>
+      </c>
+      <c r="AA61">
+        <v>11</v>
+      </c>
+      <c r="AB61">
+        <v>10</v>
+      </c>
+      <c r="AC61">
+        <f>AVERAGE(Z1:Z10)</f>
+        <v>878.21406249999995</v>
+      </c>
+    </row>
+    <row r="62" spans="2:29" ht="17.7">
       <c r="B62" s="1" t="s">
         <v>62</v>
       </c>
@@ -2370,8 +3059,17 @@
       <c r="N62">
         <v>10</v>
       </c>
-    </row>
-    <row r="63" spans="2:16" ht="17.7">
+      <c r="V62" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z62">
+        <v>0</v>
+      </c>
+      <c r="AA62">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="2:29" ht="17.7">
       <c r="B63" s="2" t="s">
         <v>63</v>
       </c>
@@ -2387,8 +3085,17 @@
       <c r="N63">
         <v>10</v>
       </c>
-    </row>
-    <row r="64" spans="2:16" ht="17.7">
+      <c r="V63" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z63">
+        <v>0</v>
+      </c>
+      <c r="AA63">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="2:29" ht="17.7">
       <c r="B64" s="2" t="s">
         <v>64</v>
       </c>
@@ -2404,8 +3111,17 @@
       <c r="N64">
         <v>21</v>
       </c>
-    </row>
-    <row r="65" spans="2:16" ht="17.7">
+      <c r="V64" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z64">
+        <v>0</v>
+      </c>
+      <c r="AA64">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="2:29" ht="17.7">
       <c r="B65" s="2" t="s">
         <v>65</v>
       </c>
@@ -2421,8 +3137,17 @@
       <c r="N65">
         <v>24</v>
       </c>
-    </row>
-    <row r="66" spans="2:16" ht="17.7">
+      <c r="V65" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z65">
+        <v>0</v>
+      </c>
+      <c r="AA65">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="2:29" ht="17.7">
       <c r="B66" s="2" t="s">
         <v>66</v>
       </c>
@@ -2438,8 +3163,17 @@
       <c r="N66">
         <v>31</v>
       </c>
-    </row>
-    <row r="67" spans="2:16" ht="17.7">
+      <c r="V66" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z66">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="AA66">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="2:29" ht="17.7">
       <c r="B67" s="2" t="s">
         <v>67</v>
       </c>
@@ -2455,8 +3189,17 @@
       <c r="N67">
         <v>35</v>
       </c>
-    </row>
-    <row r="68" spans="2:16" ht="17.7">
+      <c r="V67" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z67">
+        <v>0</v>
+      </c>
+      <c r="AA67">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="68" spans="2:29" ht="17.7">
       <c r="B68" s="2" t="s">
         <v>68</v>
       </c>
@@ -2472,8 +3215,17 @@
       <c r="N68">
         <v>43</v>
       </c>
-    </row>
-    <row r="69" spans="2:16" ht="17.7">
+      <c r="V68" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z68">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="AA68">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="69" spans="2:29" ht="17.7">
       <c r="B69" s="2" t="s">
         <v>69</v>
       </c>
@@ -2489,8 +3241,17 @@
       <c r="N69">
         <v>48</v>
       </c>
-    </row>
-    <row r="70" spans="2:16" ht="17.7">
+      <c r="V69" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="Z69">
+        <v>0</v>
+      </c>
+      <c r="AA69">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="70" spans="2:29" ht="17.7">
       <c r="B70" s="2" t="s">
         <v>70</v>
       </c>
@@ -2506,8 +3267,17 @@
       <c r="N70">
         <v>54</v>
       </c>
-    </row>
-    <row r="71" spans="2:16" ht="17.7">
+      <c r="V70" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z70">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="AA70">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="2:29" ht="17.7">
       <c r="B71" s="1" t="s">
         <v>71</v>
       </c>
@@ -2521,7 +3291,7 @@
         <v>100</v>
       </c>
       <c r="H71">
-        <f t="shared" ref="H66:H129" si="1">AVERAGE(E71:E80)</f>
+        <f t="shared" ref="H71:H121" si="1">AVERAGE(E71:E80)</f>
         <v>1.2631416320800745E-4</v>
       </c>
       <c r="M71">
@@ -2537,8 +3307,24 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="72" spans="2:16" ht="17.7">
+      <c r="V71" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Z71">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="AA71">
+        <v>107</v>
+      </c>
+      <c r="AB71">
+        <v>100</v>
+      </c>
+      <c r="AC71">
+        <f>AVERAGE(Z1:Z10)</f>
+        <v>878.21406249999995</v>
+      </c>
+    </row>
+    <row r="72" spans="2:29" ht="17.7">
       <c r="B72" s="1" t="s">
         <v>72</v>
       </c>
@@ -2554,8 +3340,17 @@
       <c r="N72">
         <v>54</v>
       </c>
-    </row>
-    <row r="73" spans="2:16" ht="17.7">
+      <c r="V72" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z72">
+        <v>3.125E-2</v>
+      </c>
+      <c r="AA72">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="2:29" ht="17.7">
       <c r="B73" s="2" t="s">
         <v>73</v>
       </c>
@@ -2571,8 +3366,17 @@
       <c r="N73">
         <v>97</v>
       </c>
-    </row>
-    <row r="74" spans="2:16" ht="17.7">
+      <c r="V73" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z73">
+        <v>1.5625E-2</v>
+      </c>
+      <c r="AA73">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="74" spans="2:29" ht="17.7">
       <c r="B74" s="2" t="s">
         <v>74</v>
       </c>
@@ -2588,8 +3392,17 @@
       <c r="N74">
         <v>142</v>
       </c>
-    </row>
-    <row r="75" spans="2:16" ht="17.7">
+      <c r="V74" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z74">
+        <v>4.6875E-2</v>
+      </c>
+      <c r="AA74">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="75" spans="2:29" ht="17.7">
       <c r="B75" s="1" t="s">
         <v>75</v>
       </c>
@@ -2605,8 +3418,17 @@
       <c r="N75">
         <v>262</v>
       </c>
-    </row>
-    <row r="76" spans="2:16" ht="17.7">
+      <c r="V75" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z75">
+        <v>4.6875E-2</v>
+      </c>
+      <c r="AA75">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="76" spans="2:29" ht="17.7">
       <c r="B76" s="1" t="s">
         <v>76</v>
       </c>
@@ -2622,8 +3444,17 @@
       <c r="N76">
         <v>279</v>
       </c>
-    </row>
-    <row r="77" spans="2:16" ht="17.7">
+      <c r="V76" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z76">
+        <v>0.609375</v>
+      </c>
+      <c r="AA76">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="77" spans="2:29" ht="17.7">
       <c r="B77" s="2" t="s">
         <v>77</v>
       </c>
@@ -2639,8 +3470,17 @@
       <c r="N77">
         <v>301</v>
       </c>
-    </row>
-    <row r="78" spans="2:16" ht="17.7">
+      <c r="V77" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="Z77">
+        <v>0.171875</v>
+      </c>
+      <c r="AA77">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="78" spans="2:29" ht="17.7">
       <c r="B78" s="2" t="s">
         <v>78</v>
       </c>
@@ -2656,8 +3496,17 @@
       <c r="N78">
         <v>410</v>
       </c>
-    </row>
-    <row r="79" spans="2:16" ht="17.7">
+      <c r="V78" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z78">
+        <v>0.671875</v>
+      </c>
+      <c r="AA78">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="79" spans="2:29" ht="17.7">
       <c r="B79" s="1" t="s">
         <v>79</v>
       </c>
@@ -2673,8 +3522,17 @@
       <c r="N79">
         <v>418</v>
       </c>
-    </row>
-    <row r="80" spans="2:16" ht="17.7">
+      <c r="V79" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z79">
+        <v>1.796875</v>
+      </c>
+      <c r="AA79">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="80" spans="2:29" ht="17.7">
       <c r="B80" s="1" t="s">
         <v>80</v>
       </c>
@@ -2690,8 +3548,17 @@
       <c r="N80">
         <v>515</v>
       </c>
-    </row>
-    <row r="81" spans="2:16" ht="17.7">
+      <c r="V80" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z80">
+        <v>3.484375</v>
+      </c>
+      <c r="AA80">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="81" spans="2:29" ht="17.7">
       <c r="B81" s="2" t="s">
         <v>81</v>
       </c>
@@ -2721,8 +3588,24 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="82" spans="2:16" ht="17.7">
+      <c r="V81" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="Z81">
+        <v>165.609375</v>
+      </c>
+      <c r="AA81">
+        <v>1001</v>
+      </c>
+      <c r="AB81">
+        <v>1000</v>
+      </c>
+      <c r="AC81">
+        <f>AVERAGE(Z1:Z10)</f>
+        <v>878.21406249999995</v>
+      </c>
+    </row>
+    <row r="82" spans="2:29" ht="17.7">
       <c r="B82" s="1" t="s">
         <v>82</v>
       </c>
@@ -2738,8 +3621,17 @@
       <c r="N82">
         <v>722</v>
       </c>
-    </row>
-    <row r="83" spans="2:16" ht="17.7">
+      <c r="V82" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z82">
+        <v>124.640625</v>
+      </c>
+      <c r="AA82">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="83" spans="2:29" ht="17.7">
       <c r="B83" s="2" t="s">
         <v>83</v>
       </c>
@@ -2755,8 +3647,17 @@
       <c r="N83">
         <v>1518</v>
       </c>
-    </row>
-    <row r="84" spans="2:16" ht="17.7">
+      <c r="V83" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="Z83">
+        <v>417.4375</v>
+      </c>
+      <c r="AA83">
+        <v>1553</v>
+      </c>
+    </row>
+    <row r="84" spans="2:29" ht="17.7">
       <c r="B84" s="2" t="s">
         <v>84</v>
       </c>
@@ -2772,8 +3673,17 @@
       <c r="N84">
         <v>1764</v>
       </c>
-    </row>
-    <row r="85" spans="2:16" ht="17.7">
+      <c r="V84" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="Z84">
+        <v>1274.609375</v>
+      </c>
+      <c r="AA84">
+        <v>2086</v>
+      </c>
+    </row>
+    <row r="85" spans="2:29" ht="17.7">
       <c r="B85" s="2" t="s">
         <v>85</v>
       </c>
@@ -2789,8 +3699,17 @@
       <c r="N85">
         <v>1699</v>
       </c>
-    </row>
-    <row r="86" spans="2:16" ht="17.7">
+      <c r="V85" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z85">
+        <v>1296.890625</v>
+      </c>
+      <c r="AA85">
+        <v>2220</v>
+      </c>
+    </row>
+    <row r="86" spans="2:29" ht="17.7">
       <c r="B86" s="2" t="s">
         <v>86</v>
       </c>
@@ -2806,8 +3725,11 @@
       <c r="N86">
         <v>2922</v>
       </c>
-    </row>
-    <row r="87" spans="2:16" ht="17.7">
+      <c r="V86" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="87" spans="2:29" ht="17.7">
       <c r="B87" s="2" t="s">
         <v>87</v>
       </c>
@@ -2823,8 +3745,11 @@
       <c r="N87">
         <v>2990</v>
       </c>
-    </row>
-    <row r="88" spans="2:16" ht="17.7">
+      <c r="V87" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="88" spans="2:29" ht="17.7">
       <c r="B88" s="2" t="s">
         <v>88</v>
       </c>
@@ -2840,8 +3765,11 @@
       <c r="N88">
         <v>2987</v>
       </c>
-    </row>
-    <row r="89" spans="2:16" ht="17.7">
+      <c r="V88" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="89" spans="2:29" ht="17.7">
       <c r="B89" s="1" t="s">
         <v>89</v>
       </c>
@@ -2857,8 +3785,11 @@
       <c r="N89">
         <v>4143</v>
       </c>
-    </row>
-    <row r="90" spans="2:16" ht="17.7">
+      <c r="V89" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="90" spans="2:29" ht="17.7">
       <c r="B90" s="1" t="s">
         <v>90</v>
       </c>
@@ -2874,8 +3805,11 @@
       <c r="N90">
         <v>4794</v>
       </c>
-    </row>
-    <row r="91" spans="2:16" ht="17.7">
+      <c r="V90" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="91" spans="2:29" ht="17.7">
       <c r="B91" s="1" t="s">
         <v>91</v>
       </c>
@@ -2905,8 +3839,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="92" spans="2:16" ht="17.7">
+      <c r="V91" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="92" spans="2:29" ht="17.7">
       <c r="B92" s="1" t="s">
         <v>92</v>
       </c>
@@ -2922,8 +3859,11 @@
       <c r="N92">
         <v>106</v>
       </c>
-    </row>
-    <row r="93" spans="2:16" ht="17.7">
+      <c r="V92" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="93" spans="2:29" ht="17.7">
       <c r="B93" s="1" t="s">
         <v>93</v>
       </c>
@@ -2939,8 +3879,11 @@
       <c r="N93">
         <v>160</v>
       </c>
-    </row>
-    <row r="94" spans="2:16" ht="17.7">
+      <c r="V93" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="94" spans="2:29" ht="17.7">
       <c r="B94" s="1" t="s">
         <v>94</v>
       </c>
@@ -2956,8 +3899,11 @@
       <c r="N94">
         <v>212</v>
       </c>
-    </row>
-    <row r="95" spans="2:16" ht="17.7">
+      <c r="V94" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="95" spans="2:29" ht="17.7">
       <c r="B95" s="1" t="s">
         <v>95</v>
       </c>
@@ -2973,8 +3919,11 @@
       <c r="N95">
         <v>273</v>
       </c>
-    </row>
-    <row r="96" spans="2:16" ht="17.7">
+      <c r="V95" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="96" spans="2:29" ht="17.7">
       <c r="B96" s="1" t="s">
         <v>96</v>
       </c>
@@ -2990,8 +3939,11 @@
       <c r="N96">
         <v>324</v>
       </c>
-    </row>
-    <row r="97" spans="2:16" ht="17.7">
+      <c r="V96" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="2:22" ht="17.7">
       <c r="B97" s="1" t="s">
         <v>97</v>
       </c>
@@ -3007,8 +3959,11 @@
       <c r="N97">
         <v>378</v>
       </c>
-    </row>
-    <row r="98" spans="2:16" ht="17.7">
+      <c r="V97" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98" spans="2:22" ht="17.7">
       <c r="B98" s="1" t="s">
         <v>98</v>
       </c>
@@ -3024,8 +3979,11 @@
       <c r="N98">
         <v>440</v>
       </c>
-    </row>
-    <row r="99" spans="2:16" ht="17.7">
+      <c r="V98" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99" spans="2:22" ht="17.7">
       <c r="B99" s="1" t="s">
         <v>99</v>
       </c>
@@ -3041,8 +3999,11 @@
       <c r="N99">
         <v>491</v>
       </c>
-    </row>
-    <row r="100" spans="2:16" ht="17.7">
+      <c r="V99" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="100" spans="2:22" ht="17.7">
       <c r="B100" s="1" t="s">
         <v>100</v>
       </c>
@@ -3058,8 +4019,11 @@
       <c r="N100">
         <v>548</v>
       </c>
-    </row>
-    <row r="101" spans="2:16" ht="17.7">
+      <c r="V100" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="101" spans="2:22" ht="17.7">
       <c r="B101" s="1" t="s">
         <v>101</v>
       </c>
@@ -3089,8 +4053,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="102" spans="2:16" ht="17.7">
+      <c r="V101" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="102" spans="2:22" ht="17.7">
       <c r="B102" s="1" t="s">
         <v>102</v>
       </c>
@@ -3106,8 +4073,11 @@
       <c r="N102">
         <v>966</v>
       </c>
-    </row>
-    <row r="103" spans="2:16" ht="17.7">
+      <c r="V102" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="103" spans="2:22" ht="17.7">
       <c r="B103" s="1" t="s">
         <v>103</v>
       </c>
@@ -3123,8 +4093,11 @@
       <c r="N103">
         <v>1473</v>
       </c>
-    </row>
-    <row r="104" spans="2:16" ht="17.7">
+      <c r="V103" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="104" spans="2:22" ht="17.7">
       <c r="B104" s="1" t="s">
         <v>104</v>
       </c>
@@ -3140,8 +4113,11 @@
       <c r="N104">
         <v>1938</v>
       </c>
-    </row>
-    <row r="105" spans="2:16" ht="17.7">
+      <c r="V104" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="105" spans="2:22" ht="17.7">
       <c r="B105" s="1" t="s">
         <v>105</v>
       </c>
@@ -3157,8 +4133,11 @@
       <c r="N105">
         <v>2537</v>
       </c>
-    </row>
-    <row r="106" spans="2:16" ht="17.7">
+      <c r="V105" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="106" spans="2:22" ht="17.7">
       <c r="B106" s="1" t="s">
         <v>106</v>
       </c>
@@ -3174,8 +4153,11 @@
       <c r="N106">
         <v>2996</v>
       </c>
-    </row>
-    <row r="107" spans="2:16" ht="17.7">
+      <c r="V106" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="107" spans="2:22" ht="17.7">
       <c r="B107" s="1" t="s">
         <v>107</v>
       </c>
@@ -3191,8 +4173,11 @@
       <c r="N107">
         <v>3366</v>
       </c>
-    </row>
-    <row r="108" spans="2:16" ht="17.7">
+      <c r="V107" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="108" spans="2:22" ht="17.7">
       <c r="B108" s="1" t="s">
         <v>108</v>
       </c>
@@ -3208,8 +4193,11 @@
       <c r="N108">
         <v>4039</v>
       </c>
-    </row>
-    <row r="109" spans="2:16" ht="17.7">
+      <c r="V108" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="109" spans="2:22" ht="17.7">
       <c r="B109" s="1" t="s">
         <v>109</v>
       </c>
@@ -3225,8 +4213,11 @@
       <c r="N109">
         <v>4442</v>
       </c>
-    </row>
-    <row r="110" spans="2:16" ht="17.7">
+      <c r="V109" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="110" spans="2:22" ht="17.7">
       <c r="B110" s="1" t="s">
         <v>110</v>
       </c>
@@ -3242,8 +4233,11 @@
       <c r="N110">
         <v>5041</v>
       </c>
-    </row>
-    <row r="111" spans="2:16" ht="17.7">
+      <c r="V110" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="111" spans="2:22" ht="17.7">
       <c r="B111" s="1" t="s">
         <v>111</v>
       </c>
@@ -3273,8 +4267,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="112" spans="2:16" ht="17.7">
+      <c r="V111" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="112" spans="2:22" ht="17.7">
       <c r="B112" s="1" t="s">
         <v>112</v>
       </c>
@@ -3290,8 +4287,11 @@
       <c r="N112">
         <v>9577</v>
       </c>
-    </row>
-    <row r="113" spans="2:16" ht="17.7">
+      <c r="V112" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="113" spans="2:22" ht="17.7">
       <c r="B113" s="1" t="s">
         <v>113</v>
       </c>
@@ -3307,8 +4307,11 @@
       <c r="N113">
         <v>14048</v>
       </c>
-    </row>
-    <row r="114" spans="2:16" ht="17.7">
+      <c r="V113" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="114" spans="2:22" ht="17.7">
       <c r="B114" s="1" t="s">
         <v>114</v>
       </c>
@@ -3324,8 +4327,11 @@
       <c r="N114">
         <v>19625</v>
       </c>
-    </row>
-    <row r="115" spans="2:16" ht="17.7">
+      <c r="V114" s="1" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="115" spans="2:22" ht="17.7">
       <c r="B115" s="1" t="s">
         <v>115</v>
       </c>
@@ -3341,8 +4347,11 @@
       <c r="N115">
         <v>24620</v>
       </c>
-    </row>
-    <row r="116" spans="2:16" ht="17.7">
+      <c r="V115" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="116" spans="2:22" ht="17.7">
       <c r="B116" s="1" t="s">
         <v>116</v>
       </c>
@@ -3358,8 +4367,11 @@
       <c r="N116">
         <v>28998</v>
       </c>
-    </row>
-    <row r="117" spans="2:16" ht="17.7">
+      <c r="V116" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="117" spans="2:22" ht="17.7">
       <c r="B117" s="1" t="s">
         <v>117</v>
       </c>
@@ -3375,8 +4387,11 @@
       <c r="N117">
         <v>33174</v>
       </c>
-    </row>
-    <row r="118" spans="2:16" ht="17.7">
+      <c r="V117" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="118" spans="2:22" ht="17.7">
       <c r="B118" s="1" t="s">
         <v>118</v>
       </c>
@@ -3392,8 +4407,11 @@
       <c r="N118">
         <v>37858</v>
       </c>
-    </row>
-    <row r="119" spans="2:16" ht="17.7">
+      <c r="V118" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="119" spans="2:22" ht="17.7">
       <c r="B119" s="1" t="s">
         <v>119</v>
       </c>
@@ -3409,8 +4427,11 @@
       <c r="N119">
         <v>44497</v>
       </c>
-    </row>
-    <row r="120" spans="2:16" ht="17.7">
+      <c r="V119" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="120" spans="2:22" ht="17.7">
       <c r="B120" s="1" t="s">
         <v>120</v>
       </c>
@@ -3426,8 +4447,11 @@
       <c r="N120">
         <v>48294</v>
       </c>
-    </row>
-    <row r="121" spans="2:16" ht="17.7">
+      <c r="V120" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="121" spans="2:22" ht="17.7">
       <c r="B121" s="2" t="s">
         <v>121</v>
       </c>
@@ -3457,8 +4481,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="122" spans="2:16" ht="17.7">
+      <c r="V121" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="122" spans="2:22" ht="17.7">
       <c r="B122" s="2" t="s">
         <v>122</v>
       </c>
@@ -3474,8 +4501,11 @@
       <c r="N122">
         <v>11</v>
       </c>
-    </row>
-    <row r="123" spans="2:16" ht="17.7">
+      <c r="V122" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="123" spans="2:22" ht="17.7">
       <c r="B123" s="2" t="s">
         <v>123</v>
       </c>
@@ -3491,8 +4521,11 @@
       <c r="N123">
         <v>11</v>
       </c>
-    </row>
-    <row r="124" spans="2:16" ht="17.7">
+      <c r="V123" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="124" spans="2:22" ht="17.7">
       <c r="B124" s="2" t="s">
         <v>124</v>
       </c>
@@ -3508,8 +4541,11 @@
       <c r="N124">
         <v>11</v>
       </c>
-    </row>
-    <row r="125" spans="2:16" ht="17.7">
+      <c r="V124" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="125" spans="2:22" ht="17.7">
       <c r="B125" s="2" t="s">
         <v>125</v>
       </c>
@@ -3525,8 +4561,11 @@
       <c r="N125">
         <v>10</v>
       </c>
-    </row>
-    <row r="126" spans="2:16" ht="17.7">
+      <c r="V125" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="126" spans="2:22" ht="17.7">
       <c r="B126" s="2" t="s">
         <v>126</v>
       </c>
@@ -3542,8 +4581,11 @@
       <c r="N126">
         <v>11</v>
       </c>
-    </row>
-    <row r="127" spans="2:16" ht="17.7">
+      <c r="V126" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="127" spans="2:22" ht="17.7">
       <c r="B127" s="2" t="s">
         <v>127</v>
       </c>
@@ -3559,8 +4601,11 @@
       <c r="N127">
         <v>11</v>
       </c>
-    </row>
-    <row r="128" spans="2:16" ht="17.7">
+      <c r="V127" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="128" spans="2:22" ht="17.7">
       <c r="B128" s="2" t="s">
         <v>128</v>
       </c>
@@ -3576,8 +4621,11 @@
       <c r="N128">
         <v>10</v>
       </c>
-    </row>
-    <row r="129" spans="2:16" ht="17.7">
+      <c r="V128" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="129" spans="2:22" ht="17.7">
       <c r="B129" s="2" t="s">
         <v>129</v>
       </c>
@@ -3593,8 +4641,11 @@
       <c r="N129">
         <v>11</v>
       </c>
-    </row>
-    <row r="130" spans="2:16" ht="17.7">
+      <c r="V129" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="130" spans="2:22" ht="17.7">
       <c r="B130" s="2" t="s">
         <v>130</v>
       </c>
@@ -3610,8 +4661,11 @@
       <c r="N130">
         <v>8</v>
       </c>
-    </row>
-    <row r="131" spans="2:16" ht="17.7">
+      <c r="V130" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="131" spans="2:22" ht="17.7">
       <c r="B131" s="2" t="s">
         <v>131</v>
       </c>
@@ -3625,7 +4679,7 @@
         <v>100</v>
       </c>
       <c r="H131">
-        <f t="shared" ref="H130:H193" si="2">AVERAGE(E131:E140)</f>
+        <f t="shared" ref="H131:H191" si="2">AVERAGE(E131:E140)</f>
         <v>4.9018859863281194E-5</v>
       </c>
       <c r="M131">
@@ -3641,8 +4695,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="132" spans="2:16" ht="17.7">
+      <c r="V131" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="132" spans="2:22" ht="17.7">
       <c r="B132" s="2" t="s">
         <v>132</v>
       </c>
@@ -3658,8 +4715,11 @@
       <c r="N132">
         <v>66</v>
       </c>
-    </row>
-    <row r="133" spans="2:16" ht="17.7">
+      <c r="V132" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="133" spans="2:22" ht="17.7">
       <c r="B133" s="2" t="s">
         <v>133</v>
       </c>
@@ -3675,8 +4735,11 @@
       <c r="N133">
         <v>34</v>
       </c>
-    </row>
-    <row r="134" spans="2:16" ht="17.7">
+      <c r="V133" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="134" spans="2:22" ht="17.7">
       <c r="B134" s="2" t="s">
         <v>134</v>
       </c>
@@ -3692,8 +4755,11 @@
       <c r="N134">
         <v>44</v>
       </c>
-    </row>
-    <row r="135" spans="2:16" ht="17.7">
+      <c r="V134" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="135" spans="2:22" ht="17.7">
       <c r="B135" s="2" t="s">
         <v>135</v>
       </c>
@@ -3709,8 +4775,11 @@
       <c r="N135">
         <v>28</v>
       </c>
-    </row>
-    <row r="136" spans="2:16" ht="17.7">
+      <c r="V135" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="136" spans="2:22" ht="17.7">
       <c r="B136" s="2" t="s">
         <v>136</v>
       </c>
@@ -3726,8 +4795,11 @@
       <c r="N136">
         <v>95</v>
       </c>
-    </row>
-    <row r="137" spans="2:16" ht="17.7">
+      <c r="V136" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="137" spans="2:22" ht="17.7">
       <c r="B137" s="2" t="s">
         <v>137</v>
       </c>
@@ -3743,8 +4815,11 @@
       <c r="N137">
         <v>72</v>
       </c>
-    </row>
-    <row r="138" spans="2:16" ht="17.7">
+      <c r="V137" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="138" spans="2:22" ht="17.7">
       <c r="B138" s="2" t="s">
         <v>138</v>
       </c>
@@ -3760,8 +4835,11 @@
       <c r="N138">
         <v>40</v>
       </c>
-    </row>
-    <row r="139" spans="2:16" ht="17.7">
+      <c r="V138" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="139" spans="2:22" ht="17.7">
       <c r="B139" s="2" t="s">
         <v>139</v>
       </c>
@@ -3777,8 +4855,11 @@
       <c r="N139">
         <v>28</v>
       </c>
-    </row>
-    <row r="140" spans="2:16" ht="17.7">
+      <c r="V139" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="140" spans="2:22" ht="17.7">
       <c r="B140" s="2" t="s">
         <v>140</v>
       </c>
@@ -3794,8 +4875,11 @@
       <c r="N140">
         <v>35</v>
       </c>
-    </row>
-    <row r="141" spans="2:16" ht="17.7">
+      <c r="V140" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="141" spans="2:22" ht="17.7">
       <c r="B141" s="2" t="s">
         <v>141</v>
       </c>
@@ -3825,8 +4909,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="142" spans="2:16" ht="17.7">
+      <c r="V141" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="142" spans="2:22" ht="17.7">
       <c r="B142" s="2" t="s">
         <v>142</v>
       </c>
@@ -3842,8 +4929,11 @@
       <c r="N142">
         <v>897</v>
       </c>
-    </row>
-    <row r="143" spans="2:16" ht="17.7">
+      <c r="V142" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="143" spans="2:22" ht="17.7">
       <c r="B143" s="2" t="s">
         <v>143</v>
       </c>
@@ -3859,8 +4949,11 @@
       <c r="N143">
         <v>676</v>
       </c>
-    </row>
-    <row r="144" spans="2:16" ht="17.7">
+      <c r="V143" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="144" spans="2:22" ht="17.7">
       <c r="B144" s="2" t="s">
         <v>144</v>
       </c>
@@ -3876,8 +4969,11 @@
       <c r="N144">
         <v>437</v>
       </c>
-    </row>
-    <row r="145" spans="2:16" ht="17.7">
+      <c r="V144" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="145" spans="2:22" ht="17.7">
       <c r="B145" s="2" t="s">
         <v>145</v>
       </c>
@@ -3893,8 +4989,11 @@
       <c r="N145">
         <v>940</v>
       </c>
-    </row>
-    <row r="146" spans="2:16" ht="17.7">
+      <c r="V145" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="146" spans="2:22" ht="17.7">
       <c r="B146" s="2" t="s">
         <v>146</v>
       </c>
@@ -3910,8 +5009,11 @@
       <c r="N146">
         <v>730</v>
       </c>
-    </row>
-    <row r="147" spans="2:16" ht="17.7">
+      <c r="V146" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="147" spans="2:22" ht="17.7">
       <c r="B147" s="2" t="s">
         <v>147</v>
       </c>
@@ -3927,8 +5029,11 @@
       <c r="N147">
         <v>307</v>
       </c>
-    </row>
-    <row r="148" spans="2:16" ht="17.7">
+      <c r="V147" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="148" spans="2:22" ht="17.7">
       <c r="B148" s="2" t="s">
         <v>148</v>
       </c>
@@ -3944,8 +5049,11 @@
       <c r="N148">
         <v>907</v>
       </c>
-    </row>
-    <row r="149" spans="2:16" ht="17.7">
+      <c r="V148" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="149" spans="2:22" ht="17.7">
       <c r="B149" s="2" t="s">
         <v>149</v>
       </c>
@@ -3961,8 +5069,11 @@
       <c r="N149">
         <v>869</v>
       </c>
-    </row>
-    <row r="150" spans="2:16" ht="17.7">
+      <c r="V149" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="150" spans="2:22" ht="17.7">
       <c r="B150" s="2" t="s">
         <v>150</v>
       </c>
@@ -3978,8 +5089,11 @@
       <c r="N150">
         <v>845</v>
       </c>
-    </row>
-    <row r="151" spans="2:16" ht="17.7">
+      <c r="V150" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="151" spans="2:22" ht="17.7">
       <c r="B151" s="1" t="s">
         <v>151</v>
       </c>
@@ -4009,8 +5123,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="152" spans="2:16" ht="17.7">
+      <c r="V151" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="152" spans="2:22" ht="17.7">
       <c r="B152" s="1" t="s">
         <v>152</v>
       </c>
@@ -4026,8 +5143,11 @@
       <c r="N152">
         <v>12</v>
       </c>
-    </row>
-    <row r="153" spans="2:16" ht="17.7">
+      <c r="V152" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="153" spans="2:22" ht="17.7">
       <c r="B153" s="1" t="s">
         <v>153</v>
       </c>
@@ -4043,8 +5163,11 @@
       <c r="N153">
         <v>32</v>
       </c>
-    </row>
-    <row r="154" spans="2:16" ht="17.7">
+      <c r="V153" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="154" spans="2:22" ht="17.7">
       <c r="B154" s="1" t="s">
         <v>154</v>
       </c>
@@ -4060,8 +5183,11 @@
       <c r="N154">
         <v>43</v>
       </c>
-    </row>
-    <row r="155" spans="2:16" ht="17.7">
+      <c r="V154" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="155" spans="2:22" ht="17.7">
       <c r="B155" s="1" t="s">
         <v>155</v>
       </c>
@@ -4077,8 +5203,11 @@
       <c r="N155">
         <v>48</v>
       </c>
-    </row>
-    <row r="156" spans="2:16" ht="17.7">
+      <c r="V155" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="156" spans="2:22" ht="17.7">
       <c r="B156" s="1" t="s">
         <v>156</v>
       </c>
@@ -4094,8 +5223,11 @@
       <c r="N156">
         <v>58</v>
       </c>
-    </row>
-    <row r="157" spans="2:16" ht="17.7">
+      <c r="V156" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="157" spans="2:22" ht="17.7">
       <c r="B157" s="1" t="s">
         <v>157</v>
       </c>
@@ -4111,8 +5243,11 @@
       <c r="N157">
         <v>72</v>
       </c>
-    </row>
-    <row r="158" spans="2:16" ht="17.7">
+      <c r="V157" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="158" spans="2:22" ht="17.7">
       <c r="B158" s="1" t="s">
         <v>158</v>
       </c>
@@ -4128,8 +5263,11 @@
       <c r="N158">
         <v>86</v>
       </c>
-    </row>
-    <row r="159" spans="2:16" ht="17.7">
+      <c r="V158" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="159" spans="2:22" ht="17.7">
       <c r="B159" s="1" t="s">
         <v>159</v>
       </c>
@@ -4145,8 +5283,11 @@
       <c r="N159">
         <v>99</v>
       </c>
-    </row>
-    <row r="160" spans="2:16" ht="17.7">
+      <c r="V159" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="160" spans="2:22" ht="17.7">
       <c r="B160" s="1" t="s">
         <v>160</v>
       </c>
@@ -4162,8 +5303,11 @@
       <c r="N160">
         <v>107</v>
       </c>
-    </row>
-    <row r="161" spans="2:16" ht="17.7">
+      <c r="V160" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="161" spans="2:22" ht="17.7">
       <c r="B161" s="1" t="s">
         <v>161</v>
       </c>
@@ -4193,8 +5337,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="162" spans="2:16" ht="17.7">
+      <c r="V161" s="1" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="162" spans="2:22" ht="17.7">
       <c r="B162" s="1" t="s">
         <v>162</v>
       </c>
@@ -4210,8 +5357,11 @@
       <c r="N162">
         <v>153</v>
       </c>
-    </row>
-    <row r="163" spans="2:16" ht="17.7">
+      <c r="V162" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="163" spans="2:22" ht="17.7">
       <c r="B163" s="1" t="s">
         <v>163</v>
       </c>
@@ -4227,8 +5377,11 @@
       <c r="N163">
         <v>266</v>
       </c>
-    </row>
-    <row r="164" spans="2:16" ht="17.7">
+      <c r="V163" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="164" spans="2:22" ht="17.7">
       <c r="B164" s="1" t="s">
         <v>164</v>
       </c>
@@ -4244,8 +5397,11 @@
       <c r="N164">
         <v>371</v>
       </c>
-    </row>
-    <row r="165" spans="2:16" ht="17.7">
+      <c r="V164" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="165" spans="2:22" ht="17.7">
       <c r="B165" s="1" t="s">
         <v>165</v>
       </c>
@@ -4261,8 +5417,11 @@
       <c r="N165">
         <v>498</v>
       </c>
-    </row>
-    <row r="166" spans="2:16" ht="17.7">
+      <c r="V165" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="166" spans="2:22" ht="17.7">
       <c r="B166" s="1" t="s">
         <v>166</v>
       </c>
@@ -4278,8 +5437,11 @@
       <c r="N166">
         <v>537</v>
       </c>
-    </row>
-    <row r="167" spans="2:16" ht="17.7">
+      <c r="V166" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="167" spans="2:22" ht="17.7">
       <c r="B167" s="1" t="s">
         <v>167</v>
       </c>
@@ -4295,8 +5457,11 @@
       <c r="N167">
         <v>690</v>
       </c>
-    </row>
-    <row r="168" spans="2:16" ht="17.7">
+      <c r="V167" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="168" spans="2:22" ht="17.7">
       <c r="B168" s="1" t="s">
         <v>168</v>
       </c>
@@ -4312,8 +5477,11 @@
       <c r="N168">
         <v>784</v>
       </c>
-    </row>
-    <row r="169" spans="2:16" ht="17.7">
+      <c r="V168" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="169" spans="2:22" ht="17.7">
       <c r="B169" s="1" t="s">
         <v>169</v>
       </c>
@@ -4329,8 +5497,11 @@
       <c r="N169">
         <v>858</v>
       </c>
-    </row>
-    <row r="170" spans="2:16" ht="17.7">
+      <c r="V169" s="1" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="170" spans="2:22" ht="17.7">
       <c r="B170" s="1" t="s">
         <v>170</v>
       </c>
@@ -4346,8 +5517,11 @@
       <c r="N170">
         <v>1053</v>
       </c>
-    </row>
-    <row r="171" spans="2:16" ht="17.7">
+      <c r="V170" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="171" spans="2:22" ht="17.7">
       <c r="B171" s="1" t="s">
         <v>171</v>
       </c>
@@ -4377,8 +5551,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="172" spans="2:16" ht="17.7">
+      <c r="V171" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="172" spans="2:22" ht="17.7">
       <c r="B172" s="1" t="s">
         <v>172</v>
       </c>
@@ -4394,8 +5571,11 @@
       <c r="N172">
         <v>1403</v>
       </c>
-    </row>
-    <row r="173" spans="2:16" ht="17.7">
+      <c r="V172" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="173" spans="2:22" ht="17.7">
       <c r="B173" s="1" t="s">
         <v>173</v>
       </c>
@@ -4411,8 +5591,11 @@
       <c r="N173">
         <v>4011</v>
       </c>
-    </row>
-    <row r="174" spans="2:16" ht="17.7">
+      <c r="V173" s="1" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="174" spans="2:22" ht="17.7">
       <c r="B174" s="1" t="s">
         <v>174</v>
       </c>
@@ -4428,8 +5611,11 @@
       <c r="N174">
         <v>3319</v>
       </c>
-    </row>
-    <row r="175" spans="2:16" ht="17.7">
+      <c r="V174" s="1" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="175" spans="2:22" ht="17.7">
       <c r="B175" s="1" t="s">
         <v>175</v>
       </c>
@@ -4445,8 +5631,11 @@
       <c r="N175">
         <v>4773</v>
       </c>
-    </row>
-    <row r="176" spans="2:16" ht="17.7">
+      <c r="V175" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="176" spans="2:22" ht="17.7">
       <c r="B176" s="1" t="s">
         <v>176</v>
       </c>
@@ -4462,8 +5651,11 @@
       <c r="N176">
         <v>5399</v>
       </c>
-    </row>
-    <row r="177" spans="2:16" ht="17.7">
+      <c r="V176" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="177" spans="2:22" ht="17.7">
       <c r="B177" s="1" t="s">
         <v>177</v>
       </c>
@@ -4479,8 +5671,11 @@
       <c r="N177">
         <v>6089</v>
       </c>
-    </row>
-    <row r="178" spans="2:16" ht="17.7">
+      <c r="V177" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="178" spans="2:22" ht="17.7">
       <c r="B178" s="1" t="s">
         <v>178</v>
       </c>
@@ -4496,8 +5691,11 @@
       <c r="N178">
         <v>6958</v>
       </c>
-    </row>
-    <row r="179" spans="2:16" ht="17.7">
+      <c r="V178" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="179" spans="2:22" ht="17.7">
       <c r="B179" s="1" t="s">
         <v>179</v>
       </c>
@@ -4513,8 +5711,11 @@
       <c r="N179">
         <v>9233</v>
       </c>
-    </row>
-    <row r="180" spans="2:16" ht="17.7">
+      <c r="V179" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="180" spans="2:22" ht="17.7">
       <c r="B180" s="1" t="s">
         <v>180</v>
       </c>
@@ -4530,8 +5731,11 @@
       <c r="N180">
         <v>9071</v>
       </c>
-    </row>
-    <row r="181" spans="2:16" ht="17.7">
+      <c r="V180" s="1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="181" spans="2:22" ht="17.7">
       <c r="B181" s="1" t="s">
         <v>181</v>
       </c>
@@ -4561,8 +5765,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="182" spans="2:16" ht="17.7">
+      <c r="V181" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="182" spans="2:22" ht="17.7">
       <c r="B182" s="1" t="s">
         <v>182</v>
       </c>
@@ -4578,8 +5785,11 @@
       <c r="N182">
         <v>218</v>
       </c>
-    </row>
-    <row r="183" spans="2:16" ht="17.7">
+      <c r="V182" s="1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="183" spans="2:22" ht="17.7">
       <c r="B183" s="1" t="s">
         <v>183</v>
       </c>
@@ -4595,8 +5805,11 @@
       <c r="N183">
         <v>325</v>
       </c>
-    </row>
-    <row r="184" spans="2:16" ht="17.7">
+      <c r="V183" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="184" spans="2:22" ht="17.7">
       <c r="B184" s="1" t="s">
         <v>184</v>
       </c>
@@ -4612,8 +5825,11 @@
       <c r="N184">
         <v>439</v>
       </c>
-    </row>
-    <row r="185" spans="2:16" ht="17.7">
+      <c r="V184" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="185" spans="2:22" ht="17.7">
       <c r="B185" s="1" t="s">
         <v>185</v>
       </c>
@@ -4629,8 +5845,11 @@
       <c r="N185">
         <v>543</v>
       </c>
-    </row>
-    <row r="186" spans="2:16" ht="17.7">
+      <c r="V185" s="1" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="186" spans="2:22" ht="17.7">
       <c r="B186" s="1" t="s">
         <v>186</v>
       </c>
@@ -4646,8 +5865,11 @@
       <c r="N186">
         <v>646</v>
       </c>
-    </row>
-    <row r="187" spans="2:16" ht="17.7">
+      <c r="V186" s="1" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="187" spans="2:22" ht="17.7">
       <c r="B187" s="1" t="s">
         <v>187</v>
       </c>
@@ -4663,8 +5885,11 @@
       <c r="N187">
         <v>882</v>
       </c>
-    </row>
-    <row r="188" spans="2:16" ht="17.7">
+      <c r="V187" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="188" spans="2:22" ht="17.7">
       <c r="B188" s="1" t="s">
         <v>188</v>
       </c>
@@ -4680,8 +5905,11 @@
       <c r="N188">
         <v>871</v>
       </c>
-    </row>
-    <row r="189" spans="2:16" ht="17.7">
+      <c r="V188" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="189" spans="2:22" ht="17.7">
       <c r="B189" s="1" t="s">
         <v>189</v>
       </c>
@@ -4697,8 +5925,11 @@
       <c r="N189">
         <v>967</v>
       </c>
-    </row>
-    <row r="190" spans="2:16" ht="17.7">
+      <c r="V189" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="190" spans="2:22" ht="17.7">
       <c r="B190" s="1" t="s">
         <v>190</v>
       </c>
@@ -4714,8 +5945,11 @@
       <c r="N190">
         <v>1104</v>
       </c>
-    </row>
-    <row r="191" spans="2:16" ht="17.7">
+      <c r="V190" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="191" spans="2:22" ht="17.7">
       <c r="B191" s="1" t="s">
         <v>191</v>
       </c>
@@ -4745,8 +5979,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="192" spans="2:16" ht="17.7">
+      <c r="V191" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="192" spans="2:22" ht="17.7">
       <c r="B192" s="1" t="s">
         <v>192</v>
       </c>
@@ -4762,8 +5999,11 @@
       <c r="N192">
         <v>1976</v>
       </c>
-    </row>
-    <row r="193" spans="2:16" ht="17.7">
+      <c r="V192" s="1" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="193" spans="2:22" ht="17.7">
       <c r="B193" s="1" t="s">
         <v>193</v>
       </c>
@@ -4779,8 +6019,11 @@
       <c r="N193">
         <v>2888</v>
       </c>
-    </row>
-    <row r="194" spans="2:16" ht="17.7">
+      <c r="V193" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="194" spans="2:22" ht="17.7">
       <c r="B194" s="1" t="s">
         <v>194</v>
       </c>
@@ -4796,8 +6039,11 @@
       <c r="N194">
         <v>3984</v>
       </c>
-    </row>
-    <row r="195" spans="2:16" ht="17.7">
+      <c r="V194" s="1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="195" spans="2:22" ht="17.7">
       <c r="B195" s="1" t="s">
         <v>195</v>
       </c>
@@ -4813,8 +6059,11 @@
       <c r="N195">
         <v>4997</v>
       </c>
-    </row>
-    <row r="196" spans="2:16" ht="17.7">
+      <c r="V195" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="196" spans="2:22" ht="17.7">
       <c r="B196" s="1" t="s">
         <v>196</v>
       </c>
@@ -4830,8 +6079,11 @@
       <c r="N196">
         <v>5998</v>
       </c>
-    </row>
-    <row r="197" spans="2:16" ht="17.7">
+      <c r="V196" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="197" spans="2:22" ht="17.7">
       <c r="B197" s="1" t="s">
         <v>197</v>
       </c>
@@ -4847,8 +6099,11 @@
       <c r="N197">
         <v>6805</v>
       </c>
-    </row>
-    <row r="198" spans="2:16" ht="17.7">
+      <c r="V197" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="198" spans="2:22" ht="17.7">
       <c r="B198" s="1" t="s">
         <v>198</v>
       </c>
@@ -4864,8 +6119,11 @@
       <c r="N198">
         <v>8134</v>
       </c>
-    </row>
-    <row r="199" spans="2:16" ht="17.7">
+      <c r="V198" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="199" spans="2:22" ht="17.7">
       <c r="B199" s="1" t="s">
         <v>199</v>
       </c>
@@ -4881,8 +6139,11 @@
       <c r="N199">
         <v>9202</v>
       </c>
-    </row>
-    <row r="200" spans="2:16" ht="17.7">
+      <c r="V199" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="200" spans="2:22" ht="17.7">
       <c r="B200" s="1" t="s">
         <v>200</v>
       </c>
@@ -4898,8 +6159,11 @@
       <c r="N200">
         <v>10202</v>
       </c>
-    </row>
-    <row r="201" spans="2:16" ht="17.7">
+      <c r="V200" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="201" spans="2:22" ht="17.7">
       <c r="B201" s="1" t="s">
         <v>201</v>
       </c>
@@ -4913,7 +6177,7 @@
         <v>1000</v>
       </c>
       <c r="H201">
-        <f t="shared" ref="H194:H211" si="3">AVERAGE(E201:E210)</f>
+        <f t="shared" ref="H201" si="3">AVERAGE(E201:E210)</f>
         <v>2.1454572677612259E-3</v>
       </c>
       <c r="M201">
@@ -4929,8 +6193,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="202" spans="2:16" ht="17.7">
+      <c r="V201" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="202" spans="2:22" ht="17.7">
       <c r="B202" s="1" t="s">
         <v>202</v>
       </c>
@@ -4946,8 +6213,11 @@
       <c r="N202">
         <v>19291</v>
       </c>
-    </row>
-    <row r="203" spans="2:16" ht="17.7">
+      <c r="V202" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="203" spans="2:22" ht="17.7">
       <c r="B203" s="1" t="s">
         <v>203</v>
       </c>
@@ -4963,8 +6233,11 @@
       <c r="N203">
         <v>28788</v>
       </c>
-    </row>
-    <row r="204" spans="2:16" ht="17.7">
+      <c r="V203" s="1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="204" spans="2:22" ht="17.7">
       <c r="B204" s="1" t="s">
         <v>204</v>
       </c>
@@ -4980,8 +6253,11 @@
       <c r="N204">
         <v>38854</v>
       </c>
-    </row>
-    <row r="205" spans="2:16" ht="17.7">
+      <c r="V204" s="1" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="205" spans="2:22" ht="17.7">
       <c r="B205" s="1" t="s">
         <v>205</v>
       </c>
@@ -4997,8 +6273,11 @@
       <c r="N205">
         <v>49957</v>
       </c>
-    </row>
-    <row r="206" spans="2:16" ht="17.7">
+      <c r="V205" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="206" spans="2:22" ht="17.7">
       <c r="B206" s="1" t="s">
         <v>206</v>
       </c>
@@ -5014,8 +6293,11 @@
       <c r="N206">
         <v>59308</v>
       </c>
-    </row>
-    <row r="207" spans="2:16" ht="17.7">
+      <c r="V206" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="207" spans="2:22" ht="17.7">
       <c r="B207" s="1" t="s">
         <v>207</v>
       </c>
@@ -5031,8 +6313,11 @@
       <c r="N207">
         <v>69155</v>
       </c>
-    </row>
-    <row r="208" spans="2:16" ht="17.7">
+      <c r="V207" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="208" spans="2:22" ht="17.7">
       <c r="B208" s="1" t="s">
         <v>208</v>
       </c>
@@ -5048,8 +6333,11 @@
       <c r="N208">
         <v>77716</v>
       </c>
-    </row>
-    <row r="209" spans="2:16" ht="17.7">
+      <c r="V208" s="1" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="209" spans="2:22" ht="17.7">
       <c r="B209" s="1" t="s">
         <v>209</v>
       </c>
@@ -5065,8 +6353,11 @@
       <c r="N209">
         <v>89704</v>
       </c>
-    </row>
-    <row r="210" spans="2:16" ht="17.7">
+      <c r="V209" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="210" spans="2:22" ht="17.7">
       <c r="B210" s="1" t="s">
         <v>210</v>
       </c>
@@ -5082,8 +6373,11 @@
       <c r="N210">
         <v>99220</v>
       </c>
-    </row>
-    <row r="211" spans="2:16" ht="17.7">
+      <c r="V210" s="1" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="211" spans="2:22" ht="17.7">
       <c r="B211" s="2" t="s">
         <v>211</v>
       </c>
@@ -5113,8 +6407,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="212" spans="2:16" ht="17.7">
+      <c r="V211" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="212" spans="2:22" ht="17.7">
       <c r="B212" s="2" t="s">
         <v>212</v>
       </c>
@@ -5131,8 +6428,11 @@
       <c r="N212">
         <v>3</v>
       </c>
-    </row>
-    <row r="213" spans="2:16" ht="17.7">
+      <c r="V212" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="213" spans="2:22" ht="17.7">
       <c r="B213" s="2" t="s">
         <v>213</v>
       </c>
@@ -5149,8 +6449,11 @@
       <c r="N213">
         <v>6</v>
       </c>
-    </row>
-    <row r="214" spans="2:16" ht="17.7">
+      <c r="V213" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="214" spans="2:22" ht="17.7">
       <c r="B214" s="2" t="s">
         <v>214</v>
       </c>
@@ -5167,8 +6470,11 @@
       <c r="N214">
         <v>7</v>
       </c>
-    </row>
-    <row r="215" spans="2:16" ht="17.7">
+      <c r="V214" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="215" spans="2:22" ht="17.7">
       <c r="B215" s="2" t="s">
         <v>215</v>
       </c>
@@ -5185,8 +6491,11 @@
       <c r="N215">
         <v>14</v>
       </c>
-    </row>
-    <row r="216" spans="2:16" ht="17.7">
+      <c r="V215" s="2" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="216" spans="2:22" ht="17.7">
       <c r="B216" s="2" t="s">
         <v>216</v>
       </c>
@@ -5203,8 +6512,11 @@
       <c r="N216">
         <v>11</v>
       </c>
-    </row>
-    <row r="217" spans="2:16" ht="17.7">
+      <c r="V216" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="217" spans="2:22" ht="17.7">
       <c r="B217" s="2" t="s">
         <v>217</v>
       </c>
@@ -5221,8 +6533,11 @@
       <c r="N217">
         <v>13</v>
       </c>
-    </row>
-    <row r="218" spans="2:16" ht="17.7">
+      <c r="V217" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="218" spans="2:22" ht="17.7">
       <c r="B218" s="2" t="s">
         <v>218</v>
       </c>
@@ -5239,8 +6554,11 @@
       <c r="N218">
         <v>20</v>
       </c>
-    </row>
-    <row r="219" spans="2:16" ht="17.7">
+      <c r="V218" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="219" spans="2:22" ht="17.7">
       <c r="B219" s="1" t="s">
         <v>219</v>
       </c>
@@ -5257,8 +6575,11 @@
       <c r="N219">
         <v>27</v>
       </c>
-    </row>
-    <row r="220" spans="2:16" ht="17.7">
+      <c r="V219" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="220" spans="2:22" ht="17.7">
       <c r="B220" s="2" t="s">
         <v>220</v>
       </c>
@@ -5275,8 +6596,11 @@
       <c r="N220">
         <v>23</v>
       </c>
-    </row>
-    <row r="221" spans="2:16" ht="17.7">
+      <c r="V220" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="221" spans="2:22" ht="17.7">
       <c r="B221" s="2" t="s">
         <v>221</v>
       </c>
@@ -5290,7 +6614,7 @@
         <v>100</v>
       </c>
       <c r="H221" s="3">
-        <f t="shared" ref="H212:H270" si="4">AVERAGE(E221:E230)</f>
+        <f t="shared" ref="H221:H261" si="4">AVERAGE(E221:E230)</f>
         <v>6.480216979980465E-5</v>
       </c>
       <c r="M221" s="3">
@@ -5306,8 +6630,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="222" spans="2:16" ht="17.7">
+      <c r="V221" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="222" spans="2:22" ht="17.7">
       <c r="B222" s="2" t="s">
         <v>222</v>
       </c>
@@ -5324,8 +6651,11 @@
       <c r="N222">
         <v>94</v>
       </c>
-    </row>
-    <row r="223" spans="2:16" ht="17.7">
+      <c r="V222" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="223" spans="2:22" ht="17.7">
       <c r="B223" s="2" t="s">
         <v>223</v>
       </c>
@@ -5342,8 +6672,11 @@
       <c r="N223">
         <v>82</v>
       </c>
-    </row>
-    <row r="224" spans="2:16" ht="17.7">
+      <c r="V223" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="224" spans="2:22" ht="17.7">
       <c r="B224" s="2" t="s">
         <v>224</v>
       </c>
@@ -5360,8 +6693,11 @@
       <c r="N224">
         <v>83</v>
       </c>
-    </row>
-    <row r="225" spans="2:16" ht="17.7">
+      <c r="V224" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="225" spans="2:22" ht="17.7">
       <c r="B225" s="2" t="s">
         <v>225</v>
       </c>
@@ -5378,8 +6714,11 @@
       <c r="N225">
         <v>64</v>
       </c>
-    </row>
-    <row r="226" spans="2:16" ht="17.7">
+      <c r="V225" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="226" spans="2:22" ht="17.7">
       <c r="B226" s="2" t="s">
         <v>226</v>
       </c>
@@ -5396,8 +6735,11 @@
       <c r="N226">
         <v>111</v>
       </c>
-    </row>
-    <row r="227" spans="2:16" ht="17.7">
+      <c r="V226" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="227" spans="2:22" ht="17.7">
       <c r="B227" s="2" t="s">
         <v>227</v>
       </c>
@@ -5414,8 +6756,11 @@
       <c r="N227">
         <v>81</v>
       </c>
-    </row>
-    <row r="228" spans="2:16" ht="17.7">
+      <c r="V227" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="228" spans="2:22" ht="17.7">
       <c r="B228" s="2" t="s">
         <v>228</v>
       </c>
@@ -5432,8 +6777,11 @@
       <c r="N228">
         <v>185</v>
       </c>
-    </row>
-    <row r="229" spans="2:16" ht="17.7">
+      <c r="V228" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="229" spans="2:22" ht="17.7">
       <c r="B229" s="2" t="s">
         <v>229</v>
       </c>
@@ -5450,8 +6798,11 @@
       <c r="N229">
         <v>263</v>
       </c>
-    </row>
-    <row r="230" spans="2:16" ht="17.7">
+      <c r="V229" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="230" spans="2:22" ht="17.7">
       <c r="B230" s="2" t="s">
         <v>230</v>
       </c>
@@ -5468,8 +6819,11 @@
       <c r="N230">
         <v>213</v>
       </c>
-    </row>
-    <row r="231" spans="2:16" ht="17.7">
+      <c r="V230" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="231" spans="2:22" ht="17.7">
       <c r="B231" s="2" t="s">
         <v>231</v>
       </c>
@@ -5499,8 +6853,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="232" spans="2:16" ht="17.7">
+      <c r="V231" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="232" spans="2:22" ht="17.7">
       <c r="B232" s="2" t="s">
         <v>232</v>
       </c>
@@ -5517,8 +6874,11 @@
       <c r="N232">
         <v>749</v>
       </c>
-    </row>
-    <row r="233" spans="2:16" ht="17.7">
+      <c r="V232" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="233" spans="2:22" ht="17.7">
       <c r="B233" s="2" t="s">
         <v>233</v>
       </c>
@@ -5535,8 +6895,11 @@
       <c r="N233">
         <v>673</v>
       </c>
-    </row>
-    <row r="234" spans="2:16" ht="17.7">
+      <c r="V233" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="234" spans="2:22" ht="17.7">
       <c r="B234" s="2" t="s">
         <v>234</v>
       </c>
@@ -5553,8 +6916,11 @@
       <c r="N234">
         <v>422</v>
       </c>
-    </row>
-    <row r="235" spans="2:16" ht="17.7">
+      <c r="V234" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="235" spans="2:22" ht="17.7">
       <c r="B235" s="2" t="s">
         <v>235</v>
       </c>
@@ -5571,8 +6937,11 @@
       <c r="N235">
         <v>238</v>
       </c>
-    </row>
-    <row r="236" spans="2:16" ht="17.7">
+      <c r="V235" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="236" spans="2:22" ht="17.7">
       <c r="B236" s="2" t="s">
         <v>236</v>
       </c>
@@ -5589,8 +6958,11 @@
       <c r="N236">
         <v>1306</v>
       </c>
-    </row>
-    <row r="237" spans="2:16" ht="17.7">
+      <c r="V236" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="237" spans="2:22" ht="17.7">
       <c r="B237" s="2" t="s">
         <v>237</v>
       </c>
@@ -5607,8 +6979,11 @@
       <c r="N237">
         <v>1717</v>
       </c>
-    </row>
-    <row r="238" spans="2:16" ht="17.7">
+      <c r="V237" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="238" spans="2:22" ht="17.7">
       <c r="B238" s="2" t="s">
         <v>238</v>
       </c>
@@ -5625,8 +7000,11 @@
       <c r="N238">
         <v>1602</v>
       </c>
-    </row>
-    <row r="239" spans="2:16" ht="17.7">
+      <c r="V238" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="239" spans="2:22" ht="17.7">
       <c r="B239" s="2" t="s">
         <v>239</v>
       </c>
@@ -5643,8 +7021,11 @@
       <c r="N239">
         <v>2253</v>
       </c>
-    </row>
-    <row r="240" spans="2:16" ht="17.7">
+      <c r="V239" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="240" spans="2:22" ht="17.7">
       <c r="B240" s="2" t="s">
         <v>240</v>
       </c>
@@ -5661,8 +7042,11 @@
       <c r="N240">
         <v>1856</v>
       </c>
-    </row>
-    <row r="241" spans="2:16" ht="17.7">
+      <c r="V240" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="241" spans="2:22" ht="17.7">
       <c r="B241" s="1" t="s">
         <v>241</v>
       </c>
@@ -5692,8 +7076,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="242" spans="2:16" ht="17.7">
+      <c r="V241" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="242" spans="2:22" ht="17.7">
       <c r="B242" s="1" t="s">
         <v>242</v>
       </c>
@@ -5710,8 +7097,11 @@
       <c r="N242">
         <v>55</v>
       </c>
-    </row>
-    <row r="243" spans="2:16" ht="17.7">
+      <c r="V242" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="243" spans="2:22" ht="17.7">
       <c r="B243" s="1" t="s">
         <v>243</v>
       </c>
@@ -5728,8 +7118,11 @@
       <c r="N243">
         <v>81</v>
       </c>
-    </row>
-    <row r="244" spans="2:16" ht="17.7">
+      <c r="V243" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="244" spans="2:22" ht="17.7">
       <c r="B244" s="1" t="s">
         <v>244</v>
       </c>
@@ -5746,8 +7139,11 @@
       <c r="N244">
         <v>107</v>
       </c>
-    </row>
-    <row r="245" spans="2:16" ht="17.7">
+      <c r="V244" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="245" spans="2:22" ht="17.7">
       <c r="B245" s="1" t="s">
         <v>245</v>
       </c>
@@ -5764,8 +7160,11 @@
       <c r="N245">
         <v>133</v>
       </c>
-    </row>
-    <row r="246" spans="2:16" ht="17.7">
+      <c r="V245" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="246" spans="2:22" ht="17.7">
       <c r="B246" s="1" t="s">
         <v>246</v>
       </c>
@@ -5782,8 +7181,11 @@
       <c r="N246">
         <v>162</v>
       </c>
-    </row>
-    <row r="247" spans="2:16" ht="17.7">
+      <c r="V246" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="247" spans="2:22" ht="17.7">
       <c r="B247" s="1" t="s">
         <v>247</v>
       </c>
@@ -5800,8 +7202,11 @@
       <c r="N247">
         <v>175</v>
       </c>
-    </row>
-    <row r="248" spans="2:16" ht="17.7">
+      <c r="V247" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="248" spans="2:22" ht="17.7">
       <c r="B248" s="1" t="s">
         <v>248</v>
       </c>
@@ -5818,8 +7223,11 @@
       <c r="N248">
         <v>213</v>
       </c>
-    </row>
-    <row r="249" spans="2:16" ht="17.7">
+      <c r="V248" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="249" spans="2:22" ht="17.7">
       <c r="B249" s="1" t="s">
         <v>249</v>
       </c>
@@ -5836,8 +7244,11 @@
       <c r="N249">
         <v>244</v>
       </c>
-    </row>
-    <row r="250" spans="2:16" ht="17.7">
+      <c r="V249" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="250" spans="2:22" ht="17.7">
       <c r="B250" s="1" t="s">
         <v>250</v>
       </c>
@@ -5854,8 +7265,11 @@
       <c r="N250">
         <v>272</v>
       </c>
-    </row>
-    <row r="251" spans="2:16" ht="17.7">
+      <c r="V250" s="1" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="251" spans="2:22" ht="17.7">
       <c r="B251" s="1" t="s">
         <v>251</v>
       </c>
@@ -5885,8 +7299,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="252" spans="2:16" ht="17.7">
+      <c r="V251" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="252" spans="2:22" ht="17.7">
       <c r="B252" s="1" t="s">
         <v>252</v>
       </c>
@@ -5903,8 +7320,11 @@
       <c r="N252">
         <v>484</v>
       </c>
-    </row>
-    <row r="253" spans="2:16" ht="17.7">
+      <c r="V252" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="253" spans="2:22" ht="17.7">
       <c r="B253" s="1" t="s">
         <v>253</v>
       </c>
@@ -5921,8 +7341,11 @@
       <c r="N253">
         <v>673</v>
       </c>
-    </row>
-    <row r="254" spans="2:16" ht="17.7">
+      <c r="V253" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="254" spans="2:22" ht="17.7">
       <c r="B254" s="1" t="s">
         <v>254</v>
       </c>
@@ -5939,8 +7362,11 @@
       <c r="N254">
         <v>928</v>
       </c>
-    </row>
-    <row r="255" spans="2:16" ht="17.7">
+      <c r="V254" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="255" spans="2:22" ht="17.7">
       <c r="B255" s="1" t="s">
         <v>255</v>
       </c>
@@ -5957,8 +7383,11 @@
       <c r="N255">
         <v>1197</v>
       </c>
-    </row>
-    <row r="256" spans="2:16" ht="17.7">
+      <c r="V255" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="256" spans="2:22" ht="17.7">
       <c r="B256" s="1" t="s">
         <v>256</v>
       </c>
@@ -5975,8 +7404,11 @@
       <c r="N256">
         <v>1492</v>
       </c>
-    </row>
-    <row r="257" spans="2:16" ht="17.7">
+      <c r="V256" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="257" spans="2:22" ht="17.7">
       <c r="B257" s="1" t="s">
         <v>257</v>
       </c>
@@ -5993,8 +7425,11 @@
       <c r="N257">
         <v>1664</v>
       </c>
-    </row>
-    <row r="258" spans="2:16" ht="17.7">
+      <c r="V257" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="258" spans="2:22" ht="17.7">
       <c r="B258" s="1" t="s">
         <v>258</v>
       </c>
@@ -6011,8 +7446,11 @@
       <c r="N258">
         <v>2104</v>
       </c>
-    </row>
-    <row r="259" spans="2:16" ht="17.7">
+      <c r="V258" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="259" spans="2:22" ht="17.7">
       <c r="B259" s="1" t="s">
         <v>259</v>
       </c>
@@ -6029,8 +7467,11 @@
       <c r="N259">
         <v>2163</v>
       </c>
-    </row>
-    <row r="260" spans="2:16" ht="17.7">
+      <c r="V259" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="260" spans="2:22" ht="17.7">
       <c r="B260" s="1" t="s">
         <v>260</v>
       </c>
@@ -6047,8 +7488,11 @@
       <c r="N260">
         <v>2550</v>
       </c>
-    </row>
-    <row r="261" spans="2:16" ht="17.7">
+      <c r="V260" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="261" spans="2:22" ht="17.7">
       <c r="B261" s="1" t="s">
         <v>261</v>
       </c>
@@ -6078,8 +7522,11 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
-    </row>
-    <row r="262" spans="2:16" ht="17.7">
+      <c r="V261" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="262" spans="2:22" ht="17.7">
       <c r="B262" s="1" t="s">
         <v>262</v>
       </c>
@@ -6096,8 +7543,11 @@
       <c r="N262">
         <v>4410</v>
       </c>
-    </row>
-    <row r="263" spans="2:16" ht="17.7">
+      <c r="V262" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="263" spans="2:22" ht="17.7">
       <c r="B263" s="1" t="s">
         <v>263</v>
       </c>
@@ -6114,8 +7564,11 @@
       <c r="N263">
         <v>6830</v>
       </c>
-    </row>
-    <row r="264" spans="2:16" ht="17.7">
+      <c r="V263" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="264" spans="2:22" ht="17.7">
       <c r="B264" s="1" t="s">
         <v>264</v>
       </c>
@@ -6132,8 +7585,11 @@
       <c r="N264">
         <v>9147</v>
       </c>
-    </row>
-    <row r="265" spans="2:16" ht="17.7">
+      <c r="V264" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="265" spans="2:22" ht="17.7">
       <c r="B265" s="1" t="s">
         <v>265</v>
       </c>
@@ -6150,8 +7606,11 @@
       <c r="N265">
         <v>11469</v>
       </c>
-    </row>
-    <row r="266" spans="2:16" ht="17.7">
+      <c r="V265" s="1" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="266" spans="2:22" ht="17.7">
       <c r="B266" s="1" t="s">
         <v>266</v>
       </c>
@@ -6168,8 +7627,11 @@
       <c r="N266">
         <v>14334</v>
       </c>
-    </row>
-    <row r="267" spans="2:16" ht="17.7">
+      <c r="V266" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="267" spans="2:22" ht="17.7">
       <c r="B267" s="1" t="s">
         <v>267</v>
       </c>
@@ -6186,8 +7648,11 @@
       <c r="N267">
         <v>16053</v>
       </c>
-    </row>
-    <row r="268" spans="2:16" ht="17.7">
+      <c r="V267" s="1" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="268" spans="2:22" ht="17.7">
       <c r="B268" s="1" t="s">
         <v>268</v>
       </c>
@@ -6204,8 +7669,11 @@
       <c r="N268">
         <v>18055</v>
       </c>
-    </row>
-    <row r="269" spans="2:16" ht="17.7">
+      <c r="V268" s="1" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="269" spans="2:22" ht="17.7">
       <c r="B269" s="1" t="s">
         <v>269</v>
       </c>
@@ -6222,8 +7690,11 @@
       <c r="N269">
         <v>21815</v>
       </c>
-    </row>
-    <row r="270" spans="2:16" ht="17.7">
+      <c r="V269" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="270" spans="2:22" ht="17.7">
       <c r="B270" s="1" t="s">
         <v>270</v>
       </c>
@@ -6239,6 +7710,9 @@
       </c>
       <c r="N270">
         <v>24176</v>
+      </c>
+      <c r="V270" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
j'ai exécuté quelques fichiers, mais je supprime pcq c'est quand même trop
</commit_message>
<xml_diff>
--- a/tp2/exemple/src/result.xlsx
+++ b/tp2/exemple/src/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\01.Travaux.Poly\09.A2018\INF4705.algo\swagnalyse\tp2\exemple\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{76E7F7E6-4012-4CC7-94B8-A5A8A7A1F9EA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C75E6E45-3811-44D5-BD12-561211AFBE2B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="78" yWindow="462" windowWidth="25440" windowHeight="14502" xr2:uid="{5E1C5933-FED9-854C-841B-467E1B961C4A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="323">
   <si>
     <t>glouton</t>
   </si>
@@ -849,12 +849,30 @@
     <t>progdyn2</t>
   </si>
   <si>
+    <t>2.484375</t>
+  </si>
+  <si>
     <t>0.0</t>
   </si>
   <si>
+    <t>0.09375</t>
+  </si>
+  <si>
+    <t>0.109375</t>
+  </si>
+  <si>
+    <t>0.078125</t>
+  </si>
+  <si>
+    <t>0.0625</t>
+  </si>
+  <si>
     <t>0.015625</t>
   </si>
   <si>
+    <t>0.03125</t>
+  </si>
+  <si>
     <t>0.953125</t>
   </si>
   <si>
@@ -925,6 +943,57 @@
   </si>
   <si>
     <t>246.6875</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>2.78125</t>
+  </si>
+  <si>
+    <t>3.109375</t>
+  </si>
+  <si>
+    <t>0.453125</t>
+  </si>
+  <si>
+    <t>0.796875</t>
+  </si>
+  <si>
+    <t>2.03125</t>
+  </si>
+  <si>
+    <t>0.203125</t>
+  </si>
+  <si>
+    <t>0.296875</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>0.96875</t>
+  </si>
+  <si>
+    <t>2.609375</t>
+  </si>
+  <si>
+    <t>3.90625</t>
+  </si>
+  <si>
+    <t>6.75</t>
+  </si>
+  <si>
+    <t>9.125</t>
+  </si>
+  <si>
+    <t>16.125</t>
+  </si>
+  <si>
+    <t>15.046875</t>
+  </si>
+  <si>
+    <t>19.53125</t>
   </si>
 </sst>
 </file>
@@ -1287,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D3A866-B3F1-5D4F-A126-3B73E31B27BE}">
   <dimension ref="A1:AE270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R91" workbookViewId="0">
-      <selection activeCell="S101" sqref="S101:T101"/>
+    <sheetView tabSelected="1" topLeftCell="R157" workbookViewId="0">
+      <selection activeCell="S170" sqref="S170:T170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
@@ -1664,7 +1733,7 @@
         <v>1.6970634460449169E-4</v>
       </c>
       <c r="S11" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="T11">
         <v>403</v>
@@ -1710,7 +1779,7 @@
         <v>391</v>
       </c>
       <c r="S12" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="T12">
         <v>438</v>
@@ -1742,7 +1811,7 @@
         <v>382</v>
       </c>
       <c r="S13" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="T13">
         <v>423</v>
@@ -1774,7 +1843,7 @@
         <v>404</v>
       </c>
       <c r="S14" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="T14">
         <v>417</v>
@@ -1806,7 +1875,7 @@
         <v>397</v>
       </c>
       <c r="S15" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="T15">
         <v>458</v>
@@ -1982,7 +2051,7 @@
         <v>2.3531913757324181E-4</v>
       </c>
       <c r="S21" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="T21">
         <v>2050</v>
@@ -2028,7 +2097,7 @@
         <v>2029</v>
       </c>
       <c r="S22" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="T22">
         <v>2044</v>
@@ -2060,7 +2129,7 @@
         <v>1927</v>
       </c>
       <c r="S23" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="T23">
         <v>2016</v>
@@ -2092,7 +2161,7 @@
         <v>1991</v>
       </c>
       <c r="S24" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="X24" s="1" t="s">
         <v>24</v>
@@ -3879,7 +3948,7 @@
         <v>86</v>
       </c>
       <c r="AB86" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
     </row>
     <row r="87" spans="2:31" ht="17.7">
@@ -3993,7 +4062,7 @@
         <v>3.8821697235107367E-4</v>
       </c>
       <c r="S91" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="T91">
         <v>54</v>
@@ -4009,7 +4078,7 @@
         <v>91</v>
       </c>
       <c r="AB91" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AC91">
         <v>54</v>
@@ -4039,7 +4108,7 @@
         <v>106</v>
       </c>
       <c r="S92" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="T92">
         <v>111</v>
@@ -4048,7 +4117,7 @@
         <v>92</v>
       </c>
       <c r="AB92" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AC92">
         <v>111</v>
@@ -4071,7 +4140,7 @@
         <v>160</v>
       </c>
       <c r="S93" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="T93">
         <v>163</v>
@@ -4080,7 +4149,7 @@
         <v>93</v>
       </c>
       <c r="AB93" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AC93">
         <v>163</v>
@@ -4103,7 +4172,7 @@
         <v>212</v>
       </c>
       <c r="S94" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="T94">
         <v>218</v>
@@ -4112,7 +4181,7 @@
         <v>94</v>
       </c>
       <c r="AB94" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="AC94">
         <v>218</v>
@@ -4135,7 +4204,7 @@
         <v>273</v>
       </c>
       <c r="S95" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="T95">
         <v>275</v>
@@ -4144,7 +4213,7 @@
         <v>95</v>
       </c>
       <c r="AB95" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="AC95">
         <v>275</v>
@@ -4167,7 +4236,7 @@
         <v>324</v>
       </c>
       <c r="S96" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="T96">
         <v>324</v>
@@ -4176,7 +4245,7 @@
         <v>96</v>
       </c>
       <c r="AB96" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="AC96">
         <v>324</v>
@@ -4199,7 +4268,7 @@
         <v>378</v>
       </c>
       <c r="S97" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="T97">
         <v>379</v>
@@ -4208,7 +4277,7 @@
         <v>97</v>
       </c>
       <c r="AB97" t="s">
-        <v>293</v>
+        <v>299</v>
       </c>
       <c r="AC97">
         <v>379</v>
@@ -4231,7 +4300,7 @@
         <v>440</v>
       </c>
       <c r="S98" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="T98">
         <v>445</v>
@@ -4240,7 +4309,7 @@
         <v>98</v>
       </c>
       <c r="AB98" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="AC98">
         <v>445</v>
@@ -4263,7 +4332,7 @@
         <v>491</v>
       </c>
       <c r="S99" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="T99">
         <v>494</v>
@@ -4272,7 +4341,7 @@
         <v>99</v>
       </c>
       <c r="AB99" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="AC99">
         <v>494</v>
@@ -4295,7 +4364,7 @@
         <v>548</v>
       </c>
       <c r="S100" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="T100">
         <v>557</v>
@@ -4304,7 +4373,7 @@
         <v>100</v>
       </c>
       <c r="AB100" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="AC100">
         <v>557</v>
@@ -4341,7 +4410,7 @@
         <v>3.8821697235107367E-4</v>
       </c>
       <c r="S101" t="s">
-        <v>299</v>
+        <v>305</v>
       </c>
       <c r="T101">
         <v>1488</v>
@@ -4357,7 +4426,7 @@
         <v>101</v>
       </c>
       <c r="AB101" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="AC101">
         <v>1488</v>
@@ -4390,7 +4459,7 @@
         <v>102</v>
       </c>
       <c r="AB102" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="AC102">
         <v>3431</v>
@@ -4436,7 +4505,7 @@
         <v>104</v>
       </c>
       <c r="AB104" t="s">
-        <v>298</v>
+        <v>304</v>
       </c>
     </row>
     <row r="105" spans="2:31" ht="17.7">
@@ -4817,6 +4886,12 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
+      <c r="S121" t="s">
+        <v>275</v>
+      </c>
+      <c r="T121">
+        <v>11</v>
+      </c>
       <c r="U121">
         <v>10</v>
       </c>
@@ -4851,6 +4926,12 @@
       <c r="N122">
         <v>11</v>
       </c>
+      <c r="S122" t="s">
+        <v>275</v>
+      </c>
+      <c r="T122">
+        <v>11</v>
+      </c>
       <c r="X122" s="2" t="s">
         <v>122</v>
       </c>
@@ -4871,6 +4952,12 @@
       <c r="N123">
         <v>11</v>
       </c>
+      <c r="S123" t="s">
+        <v>275</v>
+      </c>
+      <c r="T123">
+        <v>11</v>
+      </c>
       <c r="X123" s="2" t="s">
         <v>123</v>
       </c>
@@ -4891,6 +4978,12 @@
       <c r="N124">
         <v>11</v>
       </c>
+      <c r="S124" t="s">
+        <v>275</v>
+      </c>
+      <c r="T124">
+        <v>11</v>
+      </c>
       <c r="X124" s="2" t="s">
         <v>124</v>
       </c>
@@ -4911,6 +5004,12 @@
       <c r="N125">
         <v>10</v>
       </c>
+      <c r="S125" t="s">
+        <v>275</v>
+      </c>
+      <c r="T125">
+        <v>11</v>
+      </c>
       <c r="X125" s="2" t="s">
         <v>125</v>
       </c>
@@ -4931,6 +5030,12 @@
       <c r="N126">
         <v>11</v>
       </c>
+      <c r="S126" t="s">
+        <v>275</v>
+      </c>
+      <c r="T126">
+        <v>11</v>
+      </c>
       <c r="X126" s="2" t="s">
         <v>126</v>
       </c>
@@ -4951,6 +5056,12 @@
       <c r="N127">
         <v>11</v>
       </c>
+      <c r="S127" t="s">
+        <v>275</v>
+      </c>
+      <c r="T127">
+        <v>11</v>
+      </c>
       <c r="X127" s="2" t="s">
         <v>127</v>
       </c>
@@ -4971,6 +5082,12 @@
       <c r="N128">
         <v>10</v>
       </c>
+      <c r="S128" t="s">
+        <v>275</v>
+      </c>
+      <c r="T128">
+        <v>11</v>
+      </c>
       <c r="X128" s="2" t="s">
         <v>128</v>
       </c>
@@ -4991,6 +5108,12 @@
       <c r="N129">
         <v>11</v>
       </c>
+      <c r="S129" t="s">
+        <v>275</v>
+      </c>
+      <c r="T129">
+        <v>11</v>
+      </c>
       <c r="X129" s="2" t="s">
         <v>129</v>
       </c>
@@ -5011,6 +5134,12 @@
       <c r="N130">
         <v>8</v>
       </c>
+      <c r="S130" t="s">
+        <v>275</v>
+      </c>
+      <c r="T130">
+        <v>11</v>
+      </c>
       <c r="X130" s="2" t="s">
         <v>130</v>
       </c>
@@ -5045,6 +5174,12 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
+      <c r="S131" t="s">
+        <v>275</v>
+      </c>
+      <c r="T131">
+        <v>101</v>
+      </c>
       <c r="U131">
         <v>100</v>
       </c>
@@ -5079,6 +5214,12 @@
       <c r="N132">
         <v>66</v>
       </c>
+      <c r="S132" t="s">
+        <v>280</v>
+      </c>
+      <c r="T132">
+        <v>101</v>
+      </c>
       <c r="X132" s="2" t="s">
         <v>132</v>
       </c>
@@ -5099,6 +5240,12 @@
       <c r="N133">
         <v>34</v>
       </c>
+      <c r="S133" t="s">
+        <v>275</v>
+      </c>
+      <c r="T133">
+        <v>101</v>
+      </c>
       <c r="X133" s="2" t="s">
         <v>133</v>
       </c>
@@ -5119,6 +5266,12 @@
       <c r="N134">
         <v>44</v>
       </c>
+      <c r="S134" t="s">
+        <v>275</v>
+      </c>
+      <c r="T134">
+        <v>101</v>
+      </c>
       <c r="X134" s="2" t="s">
         <v>134</v>
       </c>
@@ -5139,6 +5292,12 @@
       <c r="N135">
         <v>28</v>
       </c>
+      <c r="S135" t="s">
+        <v>275</v>
+      </c>
+      <c r="T135">
+        <v>101</v>
+      </c>
       <c r="X135" s="2" t="s">
         <v>135</v>
       </c>
@@ -5159,6 +5318,12 @@
       <c r="N136">
         <v>95</v>
       </c>
+      <c r="S136" t="s">
+        <v>280</v>
+      </c>
+      <c r="T136">
+        <v>101</v>
+      </c>
       <c r="X136" s="2" t="s">
         <v>136</v>
       </c>
@@ -5179,6 +5344,12 @@
       <c r="N137">
         <v>72</v>
       </c>
+      <c r="S137" t="s">
+        <v>280</v>
+      </c>
+      <c r="T137">
+        <v>101</v>
+      </c>
       <c r="X137" s="2" t="s">
         <v>137</v>
       </c>
@@ -5199,6 +5370,12 @@
       <c r="N138">
         <v>40</v>
       </c>
+      <c r="S138" t="s">
+        <v>275</v>
+      </c>
+      <c r="T138">
+        <v>101</v>
+      </c>
       <c r="X138" s="2" t="s">
         <v>138</v>
       </c>
@@ -5219,6 +5396,12 @@
       <c r="N139">
         <v>28</v>
       </c>
+      <c r="S139" t="s">
+        <v>280</v>
+      </c>
+      <c r="T139">
+        <v>116</v>
+      </c>
       <c r="X139" s="2" t="s">
         <v>139</v>
       </c>
@@ -5239,6 +5422,12 @@
       <c r="N140">
         <v>35</v>
       </c>
+      <c r="S140" t="s">
+        <v>275</v>
+      </c>
+      <c r="T140">
+        <v>106</v>
+      </c>
       <c r="X140" s="2" t="s">
         <v>140</v>
       </c>
@@ -5273,6 +5462,12 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
+      <c r="S141" t="s">
+        <v>306</v>
+      </c>
+      <c r="T141">
+        <v>1001</v>
+      </c>
       <c r="U141">
         <v>1000</v>
       </c>
@@ -5307,6 +5502,12 @@
       <c r="N142">
         <v>897</v>
       </c>
+      <c r="S142" t="s">
+        <v>307</v>
+      </c>
+      <c r="T142">
+        <v>1001</v>
+      </c>
       <c r="X142" s="2" t="s">
         <v>142</v>
       </c>
@@ -5327,6 +5528,12 @@
       <c r="N143">
         <v>676</v>
       </c>
+      <c r="S143" t="s">
+        <v>308</v>
+      </c>
+      <c r="T143">
+        <v>1001</v>
+      </c>
       <c r="X143" s="2" t="s">
         <v>143</v>
       </c>
@@ -5347,6 +5554,12 @@
       <c r="N144">
         <v>437</v>
       </c>
+      <c r="S144" t="s">
+        <v>309</v>
+      </c>
+      <c r="T144">
+        <v>1001</v>
+      </c>
       <c r="X144" s="2" t="s">
         <v>144</v>
       </c>
@@ -5501,6 +5714,12 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
+      <c r="S151" t="s">
+        <v>275</v>
+      </c>
+      <c r="T151">
+        <v>11</v>
+      </c>
       <c r="U151">
         <v>10</v>
       </c>
@@ -5535,6 +5754,12 @@
       <c r="N152">
         <v>12</v>
       </c>
+      <c r="S152" t="s">
+        <v>275</v>
+      </c>
+      <c r="T152">
+        <v>21</v>
+      </c>
       <c r="X152" s="1" t="s">
         <v>152</v>
       </c>
@@ -5555,6 +5780,12 @@
       <c r="N153">
         <v>32</v>
       </c>
+      <c r="S153" t="s">
+        <v>275</v>
+      </c>
+      <c r="T153">
+        <v>32</v>
+      </c>
       <c r="X153" s="1" t="s">
         <v>153</v>
       </c>
@@ -5575,6 +5806,12 @@
       <c r="N154">
         <v>43</v>
       </c>
+      <c r="S154" t="s">
+        <v>281</v>
+      </c>
+      <c r="T154">
+        <v>46</v>
+      </c>
       <c r="X154" s="1" t="s">
         <v>154</v>
       </c>
@@ -5595,6 +5832,12 @@
       <c r="N155">
         <v>48</v>
       </c>
+      <c r="S155" t="s">
+        <v>278</v>
+      </c>
+      <c r="T155">
+        <v>54</v>
+      </c>
       <c r="X155" s="1" t="s">
         <v>155</v>
       </c>
@@ -5615,6 +5858,12 @@
       <c r="N156">
         <v>58</v>
       </c>
+      <c r="S156" t="s">
+        <v>279</v>
+      </c>
+      <c r="T156">
+        <v>64</v>
+      </c>
       <c r="X156" s="1" t="s">
         <v>156</v>
       </c>
@@ -5635,6 +5884,12 @@
       <c r="N157">
         <v>72</v>
       </c>
+      <c r="S157" t="s">
+        <v>277</v>
+      </c>
+      <c r="T157">
+        <v>73</v>
+      </c>
       <c r="X157" s="1" t="s">
         <v>157</v>
       </c>
@@ -5655,6 +5910,12 @@
       <c r="N158">
         <v>86</v>
       </c>
+      <c r="S158" t="s">
+        <v>277</v>
+      </c>
+      <c r="T158">
+        <v>86</v>
+      </c>
       <c r="X158" s="1" t="s">
         <v>158</v>
       </c>
@@ -5675,6 +5936,12 @@
       <c r="N159">
         <v>99</v>
       </c>
+      <c r="S159" t="s">
+        <v>312</v>
+      </c>
+      <c r="T159">
+        <v>104</v>
+      </c>
       <c r="X159" s="1" t="s">
         <v>159</v>
       </c>
@@ -5695,6 +5962,12 @@
       <c r="N160">
         <v>107</v>
       </c>
+      <c r="S160" t="s">
+        <v>313</v>
+      </c>
+      <c r="T160">
+        <v>112</v>
+      </c>
       <c r="X160" s="1" t="s">
         <v>160</v>
       </c>
@@ -5729,6 +6002,12 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
+      <c r="S161" t="s">
+        <v>275</v>
+      </c>
+      <c r="T161">
+        <v>101</v>
+      </c>
       <c r="U161">
         <v>100</v>
       </c>
@@ -5763,6 +6042,12 @@
       <c r="N162">
         <v>153</v>
       </c>
+      <c r="S162" t="s">
+        <v>314</v>
+      </c>
+      <c r="T162">
+        <v>203</v>
+      </c>
       <c r="X162" s="1" t="s">
         <v>162</v>
       </c>
@@ -5783,6 +6068,12 @@
       <c r="N163">
         <v>266</v>
       </c>
+      <c r="S163" t="s">
+        <v>315</v>
+      </c>
+      <c r="T163">
+        <v>298</v>
+      </c>
       <c r="X163" s="1" t="s">
         <v>163</v>
       </c>
@@ -5803,6 +6094,12 @@
       <c r="N164">
         <v>371</v>
       </c>
+      <c r="S164" t="s">
+        <v>316</v>
+      </c>
+      <c r="T164">
+        <v>425</v>
+      </c>
       <c r="X164" s="1" t="s">
         <v>164</v>
       </c>
@@ -5823,6 +6120,12 @@
       <c r="N165">
         <v>498</v>
       </c>
+      <c r="S165" t="s">
+        <v>317</v>
+      </c>
+      <c r="T165">
+        <v>524</v>
+      </c>
       <c r="X165" s="1" t="s">
         <v>165</v>
       </c>
@@ -5843,6 +6146,12 @@
       <c r="N166">
         <v>537</v>
       </c>
+      <c r="S166" t="s">
+        <v>318</v>
+      </c>
+      <c r="T166">
+        <v>599</v>
+      </c>
       <c r="X166" s="1" t="s">
         <v>166</v>
       </c>
@@ -5863,6 +6172,12 @@
       <c r="N167">
         <v>690</v>
       </c>
+      <c r="S167" t="s">
+        <v>319</v>
+      </c>
+      <c r="T167">
+        <v>696</v>
+      </c>
       <c r="X167" s="1" t="s">
         <v>167</v>
       </c>
@@ -5883,6 +6198,12 @@
       <c r="N168">
         <v>784</v>
       </c>
+      <c r="S168" t="s">
+        <v>320</v>
+      </c>
+      <c r="T168">
+        <v>850</v>
+      </c>
       <c r="X168" s="1" t="s">
         <v>168</v>
       </c>
@@ -5903,6 +6224,12 @@
       <c r="N169">
         <v>858</v>
       </c>
+      <c r="S169" t="s">
+        <v>321</v>
+      </c>
+      <c r="T169">
+        <v>869</v>
+      </c>
       <c r="X169" s="1" t="s">
         <v>169</v>
       </c>
@@ -5923,6 +6250,12 @@
       <c r="N170">
         <v>1053</v>
       </c>
+      <c r="S170" t="s">
+        <v>322</v>
+      </c>
+      <c r="T170">
+        <v>1054</v>
+      </c>
       <c r="X170" s="1" t="s">
         <v>170</v>
       </c>
@@ -6869,6 +7202,12 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
+      <c r="S211" t="s">
+        <v>275</v>
+      </c>
+      <c r="T211">
+        <v>11</v>
+      </c>
       <c r="U211">
         <v>10</v>
       </c>
@@ -6904,6 +7243,12 @@
       <c r="N212">
         <v>3</v>
       </c>
+      <c r="S212" t="s">
+        <v>275</v>
+      </c>
+      <c r="T212">
+        <v>11</v>
+      </c>
       <c r="V212" s="3"/>
       <c r="X212" s="2" t="s">
         <v>212</v>
@@ -6927,6 +7272,12 @@
       <c r="N213">
         <v>6</v>
       </c>
+      <c r="S213" t="s">
+        <v>275</v>
+      </c>
+      <c r="T213">
+        <v>11</v>
+      </c>
       <c r="V213" s="3"/>
       <c r="X213" s="2" t="s">
         <v>213</v>
@@ -6950,6 +7301,12 @@
       <c r="N214">
         <v>7</v>
       </c>
+      <c r="S214" t="s">
+        <v>275</v>
+      </c>
+      <c r="T214">
+        <v>11</v>
+      </c>
       <c r="V214" s="3"/>
       <c r="X214" s="2" t="s">
         <v>214</v>
@@ -6973,6 +7330,12 @@
       <c r="N215">
         <v>14</v>
       </c>
+      <c r="S215" t="s">
+        <v>275</v>
+      </c>
+      <c r="T215">
+        <v>14</v>
+      </c>
       <c r="V215" s="3"/>
       <c r="X215" s="2" t="s">
         <v>215</v>
@@ -6996,6 +7359,12 @@
       <c r="N216">
         <v>11</v>
       </c>
+      <c r="S216" t="s">
+        <v>275</v>
+      </c>
+      <c r="T216">
+        <v>15</v>
+      </c>
       <c r="V216" s="3"/>
       <c r="X216" s="2" t="s">
         <v>216</v>
@@ -7019,6 +7388,12 @@
       <c r="N217">
         <v>13</v>
       </c>
+      <c r="S217" t="s">
+        <v>275</v>
+      </c>
+      <c r="T217">
+        <v>16</v>
+      </c>
       <c r="V217" s="3"/>
       <c r="X217" s="2" t="s">
         <v>217</v>
@@ -7042,6 +7417,12 @@
       <c r="N218">
         <v>20</v>
       </c>
+      <c r="S218" t="s">
+        <v>275</v>
+      </c>
+      <c r="T218">
+        <v>22</v>
+      </c>
       <c r="V218" s="3"/>
       <c r="X218" s="2" t="s">
         <v>218</v>
@@ -7065,6 +7446,12 @@
       <c r="N219">
         <v>27</v>
       </c>
+      <c r="S219" t="s">
+        <v>275</v>
+      </c>
+      <c r="T219">
+        <v>29</v>
+      </c>
       <c r="V219" s="3"/>
       <c r="X219" s="1" t="s">
         <v>219</v>
@@ -7088,6 +7475,12 @@
       <c r="N220">
         <v>23</v>
       </c>
+      <c r="S220" t="s">
+        <v>275</v>
+      </c>
+      <c r="T220">
+        <v>27</v>
+      </c>
       <c r="V220" s="3"/>
       <c r="X220" s="2" t="s">
         <v>220</v>
@@ -7124,6 +7517,12 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
+      <c r="S221" t="s">
+        <v>275</v>
+      </c>
+      <c r="T221">
+        <v>101</v>
+      </c>
       <c r="U221">
         <v>100</v>
       </c>
@@ -7159,6 +7558,12 @@
       <c r="N222">
         <v>94</v>
       </c>
+      <c r="S222" t="s">
+        <v>280</v>
+      </c>
+      <c r="T222">
+        <v>101</v>
+      </c>
       <c r="V222" s="3"/>
       <c r="X222" s="2" t="s">
         <v>222</v>
@@ -7182,6 +7587,12 @@
       <c r="N223">
         <v>82</v>
       </c>
+      <c r="S223" t="s">
+        <v>275</v>
+      </c>
+      <c r="T223">
+        <v>101</v>
+      </c>
       <c r="V223" s="3"/>
       <c r="X223" s="2" t="s">
         <v>223</v>
@@ -7205,6 +7616,12 @@
       <c r="N224">
         <v>83</v>
       </c>
+      <c r="S224" t="s">
+        <v>275</v>
+      </c>
+      <c r="T224">
+        <v>101</v>
+      </c>
       <c r="V224" s="3"/>
       <c r="X224" s="2" t="s">
         <v>224</v>
@@ -7228,6 +7645,12 @@
       <c r="N225">
         <v>64</v>
       </c>
+      <c r="S225" t="s">
+        <v>280</v>
+      </c>
+      <c r="T225">
+        <v>131</v>
+      </c>
       <c r="V225" s="3"/>
       <c r="X225" s="2" t="s">
         <v>225</v>
@@ -7251,6 +7674,12 @@
       <c r="N226">
         <v>111</v>
       </c>
+      <c r="S226" t="s">
+        <v>280</v>
+      </c>
+      <c r="T226">
+        <v>162</v>
+      </c>
       <c r="V226" s="3"/>
       <c r="X226" s="2" t="s">
         <v>226</v>
@@ -7274,6 +7703,12 @@
       <c r="N227">
         <v>81</v>
       </c>
+      <c r="S227" t="s">
+        <v>281</v>
+      </c>
+      <c r="T227">
+        <v>180</v>
+      </c>
       <c r="V227" s="3"/>
       <c r="X227" s="2" t="s">
         <v>227</v>
@@ -7297,6 +7732,12 @@
       <c r="N228">
         <v>185</v>
       </c>
+      <c r="S228" t="s">
+        <v>276</v>
+      </c>
+      <c r="T228">
+        <v>216</v>
+      </c>
       <c r="V228" s="3"/>
       <c r="X228" s="2" t="s">
         <v>228</v>
@@ -7320,6 +7761,12 @@
       <c r="N229">
         <v>263</v>
       </c>
+      <c r="S229" t="s">
+        <v>281</v>
+      </c>
+      <c r="T229">
+        <v>263</v>
+      </c>
       <c r="V229" s="3"/>
       <c r="X229" s="2" t="s">
         <v>229</v>
@@ -7343,6 +7790,12 @@
       <c r="N230">
         <v>213</v>
       </c>
+      <c r="S230" t="s">
+        <v>281</v>
+      </c>
+      <c r="T230">
+        <v>245</v>
+      </c>
       <c r="V230" s="3"/>
       <c r="X230" s="2" t="s">
         <v>230</v>
@@ -7379,6 +7832,12 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
+      <c r="S231" t="s">
+        <v>310</v>
+      </c>
+      <c r="T231">
+        <v>1001</v>
+      </c>
       <c r="U231">
         <v>1000</v>
       </c>
@@ -7414,6 +7873,12 @@
       <c r="N232">
         <v>749</v>
       </c>
+      <c r="S232" t="s">
+        <v>311</v>
+      </c>
+      <c r="T232">
+        <v>1001</v>
+      </c>
       <c r="V232" s="3"/>
       <c r="X232" s="2" t="s">
         <v>232</v>
@@ -7436,6 +7901,12 @@
       </c>
       <c r="N233">
         <v>673</v>
+      </c>
+      <c r="S233" t="s">
+        <v>274</v>
+      </c>
+      <c r="T233">
+        <v>1433</v>
       </c>
       <c r="V233" s="3"/>
       <c r="X233" s="2" t="s">

</xml_diff>

<commit_message>
temps pour progdyn1 reste juste une donnée
</commit_message>
<xml_diff>
--- a/tp2/exemple/src/result.xlsx
+++ b/tp2/exemple/src/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\01.Travaux.Poly\09.A2018\INF4705.algo\swagnalyse\tp2\exemple\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C75E6E45-3811-44D5-BD12-561211AFBE2B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{939EEAC4-BCF4-4C72-84A6-1882D6A06608}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="78" yWindow="462" windowWidth="25440" windowHeight="14502" xr2:uid="{5E1C5933-FED9-854C-841B-467E1B961C4A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="355">
   <si>
     <t>glouton</t>
   </si>
@@ -994,6 +994,102 @@
   </si>
   <si>
     <t>19.53125</t>
+  </si>
+  <si>
+    <t>2.59375;108</t>
+  </si>
+  <si>
+    <t>14.109375;221</t>
+  </si>
+  <si>
+    <t>32.78125;329</t>
+  </si>
+  <si>
+    <t>60.03125;440</t>
+  </si>
+  <si>
+    <t>94.0;548</t>
+  </si>
+  <si>
+    <t>133.390625;655</t>
+  </si>
+  <si>
+    <t>371.390625;885</t>
+  </si>
+  <si>
+    <t>15.734375;510</t>
+  </si>
+  <si>
+    <t>87.171875;1005</t>
+  </si>
+  <si>
+    <t>217.984375;1533</t>
+  </si>
+  <si>
+    <t>629.40625;2225</t>
+  </si>
+  <si>
+    <t>0.046875;27</t>
+  </si>
+  <si>
+    <t>0.171875;56</t>
+  </si>
+  <si>
+    <t>0.53125;82</t>
+  </si>
+  <si>
+    <t>0.875;113</t>
+  </si>
+  <si>
+    <t>1.375;135</t>
+  </si>
+  <si>
+    <t>2.40625;163</t>
+  </si>
+  <si>
+    <t>2.671875;182</t>
+  </si>
+  <si>
+    <t>3.84375;222</t>
+  </si>
+  <si>
+    <t>4.828125;247</t>
+  </si>
+  <si>
+    <t>6.109375;275</t>
+  </si>
+  <si>
+    <t>254.140625;2523</t>
+  </si>
+  <si>
+    <t>332.0;994</t>
+  </si>
+  <si>
+    <t>3491.234375;4960</t>
+  </si>
+  <si>
+    <t>1.453125;1001</t>
+  </si>
+  <si>
+    <t>108.453125;2523</t>
+  </si>
+  <si>
+    <t>128.203125;1001</t>
+  </si>
+  <si>
+    <t>5415.203125;9911</t>
+  </si>
+  <si>
+    <t>5.109375;994</t>
+  </si>
+  <si>
+    <t>92.4375;1001</t>
+  </si>
+  <si>
+    <t>45.828125;1000</t>
+  </si>
+  <si>
+    <t>641.28125;4960</t>
   </si>
 </sst>
 </file>
@@ -1046,6 +1142,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1062,10 +1226,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="FFFFFF"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="000000"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1356,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D3A866-B3F1-5D4F-A126-3B73E31B27BE}">
   <dimension ref="A1:AE270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R157" workbookViewId="0">
-      <selection activeCell="S170" sqref="S170:T170"/>
+    <sheetView tabSelected="1" topLeftCell="T97" workbookViewId="0">
+      <selection activeCell="W102" sqref="W102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
@@ -4658,6 +4822,9 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
+      <c r="S111" t="s">
+        <v>346</v>
+      </c>
       <c r="U111">
         <v>1000</v>
       </c>
@@ -4668,6 +4835,9 @@
       <c r="X111" s="1" t="s">
         <v>111</v>
       </c>
+      <c r="AB111" t="s">
+        <v>354</v>
+      </c>
       <c r="AD111">
         <v>1000</v>
       </c>
@@ -5478,6 +5648,9 @@
       <c r="X141" s="2" t="s">
         <v>141</v>
       </c>
+      <c r="AB141" t="s">
+        <v>353</v>
+      </c>
       <c r="AD141">
         <v>1000</v>
       </c>
@@ -6290,6 +6463,9 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
+      <c r="S171" t="s">
+        <v>347</v>
+      </c>
       <c r="U171">
         <v>1000</v>
       </c>
@@ -6300,6 +6476,9 @@
       <c r="X171" s="1" t="s">
         <v>171</v>
       </c>
+      <c r="AB171" t="s">
+        <v>352</v>
+      </c>
       <c r="AD171">
         <v>1000</v>
       </c>
@@ -6518,6 +6697,9 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
+      <c r="S181" t="s">
+        <v>323</v>
+      </c>
       <c r="U181">
         <v>10</v>
       </c>
@@ -6552,6 +6734,9 @@
       <c r="N182">
         <v>218</v>
       </c>
+      <c r="S182" t="s">
+        <v>324</v>
+      </c>
       <c r="X182" s="1" t="s">
         <v>182</v>
       </c>
@@ -6572,6 +6757,9 @@
       <c r="N183">
         <v>325</v>
       </c>
+      <c r="S183" t="s">
+        <v>325</v>
+      </c>
       <c r="X183" s="1" t="s">
         <v>183</v>
       </c>
@@ -6592,6 +6780,9 @@
       <c r="N184">
         <v>439</v>
       </c>
+      <c r="S184" t="s">
+        <v>326</v>
+      </c>
       <c r="X184" s="1" t="s">
         <v>184</v>
       </c>
@@ -6612,6 +6803,9 @@
       <c r="N185">
         <v>543</v>
       </c>
+      <c r="S185" t="s">
+        <v>327</v>
+      </c>
       <c r="X185" s="1" t="s">
         <v>185</v>
       </c>
@@ -6632,6 +6826,9 @@
       <c r="N186">
         <v>646</v>
       </c>
+      <c r="S186" t="s">
+        <v>328</v>
+      </c>
       <c r="X186" s="1" t="s">
         <v>186</v>
       </c>
@@ -6652,6 +6849,9 @@
       <c r="N187">
         <v>882</v>
       </c>
+      <c r="S187" t="s">
+        <v>329</v>
+      </c>
       <c r="X187" s="1" t="s">
         <v>187</v>
       </c>
@@ -6746,6 +6946,9 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
+      <c r="S191" t="s">
+        <v>345</v>
+      </c>
       <c r="U191">
         <v>100</v>
       </c>
@@ -6756,6 +6959,9 @@
       <c r="X191" s="1" t="s">
         <v>191</v>
       </c>
+      <c r="AB191" t="s">
+        <v>351</v>
+      </c>
       <c r="AD191">
         <v>100</v>
       </c>
@@ -6984,6 +7190,9 @@
       <c r="X201" s="1" t="s">
         <v>201</v>
       </c>
+      <c r="AB201" t="s">
+        <v>350</v>
+      </c>
       <c r="AD201">
         <v>1000</v>
       </c>
@@ -7848,6 +8057,9 @@
       <c r="X231" s="2" t="s">
         <v>231</v>
       </c>
+      <c r="AB231" t="s">
+        <v>349</v>
+      </c>
       <c r="AD231">
         <v>1000</v>
       </c>
@@ -8105,6 +8317,9 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
+      <c r="S241" t="s">
+        <v>334</v>
+      </c>
       <c r="U241">
         <v>10</v>
       </c>
@@ -8140,6 +8355,9 @@
       <c r="N242">
         <v>55</v>
       </c>
+      <c r="S242" t="s">
+        <v>335</v>
+      </c>
       <c r="V242" s="3"/>
       <c r="X242" s="1" t="s">
         <v>242</v>
@@ -8163,6 +8381,9 @@
       <c r="N243">
         <v>81</v>
       </c>
+      <c r="S243" t="s">
+        <v>336</v>
+      </c>
       <c r="V243" s="3"/>
       <c r="X243" s="1" t="s">
         <v>243</v>
@@ -8186,6 +8407,9 @@
       <c r="N244">
         <v>107</v>
       </c>
+      <c r="S244" t="s">
+        <v>337</v>
+      </c>
       <c r="V244" s="3"/>
       <c r="X244" s="1" t="s">
         <v>244</v>
@@ -8209,6 +8433,9 @@
       <c r="N245">
         <v>133</v>
       </c>
+      <c r="S245" t="s">
+        <v>338</v>
+      </c>
       <c r="V245" s="3"/>
       <c r="X245" s="1" t="s">
         <v>245</v>
@@ -8232,6 +8459,9 @@
       <c r="N246">
         <v>162</v>
       </c>
+      <c r="S246" t="s">
+        <v>339</v>
+      </c>
       <c r="V246" s="3"/>
       <c r="X246" s="1" t="s">
         <v>246</v>
@@ -8255,6 +8485,9 @@
       <c r="N247">
         <v>175</v>
       </c>
+      <c r="S247" t="s">
+        <v>340</v>
+      </c>
       <c r="V247" s="3"/>
       <c r="X247" s="1" t="s">
         <v>247</v>
@@ -8278,6 +8511,9 @@
       <c r="N248">
         <v>213</v>
       </c>
+      <c r="S248" t="s">
+        <v>341</v>
+      </c>
       <c r="V248" s="3"/>
       <c r="X248" s="1" t="s">
         <v>248</v>
@@ -8301,6 +8537,9 @@
       <c r="N249">
         <v>244</v>
       </c>
+      <c r="S249" t="s">
+        <v>342</v>
+      </c>
       <c r="V249" s="3"/>
       <c r="X249" s="1" t="s">
         <v>249</v>
@@ -8324,6 +8563,9 @@
       <c r="N250">
         <v>272</v>
       </c>
+      <c r="S250" t="s">
+        <v>343</v>
+      </c>
       <c r="V250" s="3"/>
       <c r="X250" s="1" t="s">
         <v>250</v>
@@ -8360,6 +8602,9 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
+      <c r="S251" t="s">
+        <v>330</v>
+      </c>
       <c r="U251">
         <v>100</v>
       </c>
@@ -8395,6 +8640,9 @@
       <c r="N252">
         <v>484</v>
       </c>
+      <c r="S252" t="s">
+        <v>331</v>
+      </c>
       <c r="V252" s="3"/>
       <c r="X252" s="1" t="s">
         <v>252</v>
@@ -8418,6 +8666,9 @@
       <c r="N253">
         <v>673</v>
       </c>
+      <c r="S253" t="s">
+        <v>332</v>
+      </c>
       <c r="V253" s="3"/>
       <c r="X253" s="1" t="s">
         <v>253</v>
@@ -8441,6 +8692,9 @@
       <c r="N254">
         <v>928</v>
       </c>
+      <c r="S254" t="s">
+        <v>333</v>
+      </c>
       <c r="V254" s="3"/>
       <c r="X254" s="1" t="s">
         <v>254</v>
@@ -8615,6 +8869,9 @@
         <f>AVERAGE(M1:M10)</f>
         <v>3.8821697235107367E-4</v>
       </c>
+      <c r="S261" t="s">
+        <v>344</v>
+      </c>
       <c r="U261">
         <v>1000</v>
       </c>
@@ -8624,6 +8881,9 @@
       </c>
       <c r="X261" s="1" t="s">
         <v>261</v>
+      </c>
+      <c r="AB261" t="s">
+        <v>348</v>
       </c>
       <c r="AD261">
         <v>1000</v>

</xml_diff>

<commit_message>
il manque les données légères et le 2000-1000 du progdyn1 (qui roule encore)
</commit_message>
<xml_diff>
--- a/tp2/exemple/src/result.xlsx
+++ b/tp2/exemple/src/result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Documents\01.Travaux.Poly\09.A2018\INF4705.algo\swagnalyse\tp2\exemple\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{939EEAC4-BCF4-4C72-84A6-1882D6A06608}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{2695E737-41F8-4DD3-90C7-E7EE8EDF2835}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="78" yWindow="462" windowWidth="25440" windowHeight="14502" xr2:uid="{5E1C5933-FED9-854C-841B-467E1B961C4A}"/>
   </bookViews>
@@ -939,9 +939,6 @@
     <t>326.453125</t>
   </si>
   <si>
-    <t>reste1</t>
-  </si>
-  <si>
     <t>246.6875</t>
   </si>
   <si>
@@ -1090,6 +1087,9 @@
   </si>
   <si>
     <t>641.28125;4960</t>
+  </si>
+  <si>
+    <t>1.0625;496</t>
   </si>
 </sst>
 </file>
@@ -1520,8 +1520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D3A866-B3F1-5D4F-A126-3B73E31B27BE}">
   <dimension ref="A1:AE270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T97" workbookViewId="0">
-      <selection activeCell="W102" sqref="W102"/>
+    <sheetView tabSelected="1" topLeftCell="T100" workbookViewId="0">
+      <selection activeCell="AB107" sqref="AB107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6"/>
@@ -4574,7 +4574,7 @@
         <v>3.8821697235107367E-4</v>
       </c>
       <c r="S101" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="T101">
         <v>1488</v>
@@ -4648,6 +4648,9 @@
       <c r="X103" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="AB103" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="104" spans="2:31" ht="17.7">
       <c r="B104" s="1" t="s">
@@ -4668,9 +4671,6 @@
       <c r="X104" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="AB104" t="s">
-        <v>304</v>
-      </c>
     </row>
     <row r="105" spans="2:31" ht="17.7">
       <c r="B105" s="1" t="s">
@@ -4823,7 +4823,7 @@
         <v>3.8821697235107367E-4</v>
       </c>
       <c r="S111" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="U111">
         <v>1000</v>
@@ -4836,7 +4836,7 @@
         <v>111</v>
       </c>
       <c r="AB111" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AD111">
         <v>1000</v>
@@ -5633,7 +5633,7 @@
         <v>3.8821697235107367E-4</v>
       </c>
       <c r="S141" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="T141">
         <v>1001</v>
@@ -5649,7 +5649,7 @@
         <v>141</v>
       </c>
       <c r="AB141" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AD141">
         <v>1000</v>
@@ -5676,7 +5676,7 @@
         <v>897</v>
       </c>
       <c r="S142" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="T142">
         <v>1001</v>
@@ -5702,7 +5702,7 @@
         <v>676</v>
       </c>
       <c r="S143" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="T143">
         <v>1001</v>
@@ -5728,7 +5728,7 @@
         <v>437</v>
       </c>
       <c r="S144" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="T144">
         <v>1001</v>
@@ -6110,7 +6110,7 @@
         <v>99</v>
       </c>
       <c r="S159" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="T159">
         <v>104</v>
@@ -6136,7 +6136,7 @@
         <v>107</v>
       </c>
       <c r="S160" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="T160">
         <v>112</v>
@@ -6216,7 +6216,7 @@
         <v>153</v>
       </c>
       <c r="S162" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="T162">
         <v>203</v>
@@ -6242,7 +6242,7 @@
         <v>266</v>
       </c>
       <c r="S163" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="T163">
         <v>298</v>
@@ -6268,7 +6268,7 @@
         <v>371</v>
       </c>
       <c r="S164" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="T164">
         <v>425</v>
@@ -6294,7 +6294,7 @@
         <v>498</v>
       </c>
       <c r="S165" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="T165">
         <v>524</v>
@@ -6320,7 +6320,7 @@
         <v>537</v>
       </c>
       <c r="S166" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="T166">
         <v>599</v>
@@ -6346,7 +6346,7 @@
         <v>690</v>
       </c>
       <c r="S167" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="T167">
         <v>696</v>
@@ -6372,7 +6372,7 @@
         <v>784</v>
       </c>
       <c r="S168" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="T168">
         <v>850</v>
@@ -6398,7 +6398,7 @@
         <v>858</v>
       </c>
       <c r="S169" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="T169">
         <v>869</v>
@@ -6424,7 +6424,7 @@
         <v>1053</v>
       </c>
       <c r="S170" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="T170">
         <v>1054</v>
@@ -6464,7 +6464,7 @@
         <v>3.8821697235107367E-4</v>
       </c>
       <c r="S171" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="U171">
         <v>1000</v>
@@ -6477,7 +6477,7 @@
         <v>171</v>
       </c>
       <c r="AB171" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AD171">
         <v>1000</v>
@@ -6698,7 +6698,7 @@
         <v>3.8821697235107367E-4</v>
       </c>
       <c r="S181" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="U181">
         <v>10</v>
@@ -6735,7 +6735,7 @@
         <v>218</v>
       </c>
       <c r="S182" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="X182" s="1" t="s">
         <v>182</v>
@@ -6758,7 +6758,7 @@
         <v>325</v>
       </c>
       <c r="S183" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="X183" s="1" t="s">
         <v>183</v>
@@ -6781,7 +6781,7 @@
         <v>439</v>
       </c>
       <c r="S184" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="X184" s="1" t="s">
         <v>184</v>
@@ -6804,7 +6804,7 @@
         <v>543</v>
       </c>
       <c r="S185" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="X185" s="1" t="s">
         <v>185</v>
@@ -6827,7 +6827,7 @@
         <v>646</v>
       </c>
       <c r="S186" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="X186" s="1" t="s">
         <v>186</v>
@@ -6850,7 +6850,7 @@
         <v>882</v>
       </c>
       <c r="S187" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="X187" s="1" t="s">
         <v>187</v>
@@ -6947,7 +6947,7 @@
         <v>3.8821697235107367E-4</v>
       </c>
       <c r="S191" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="U191">
         <v>100</v>
@@ -6960,7 +6960,7 @@
         <v>191</v>
       </c>
       <c r="AB191" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AD191">
         <v>100</v>
@@ -7191,7 +7191,7 @@
         <v>201</v>
       </c>
       <c r="AB201" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AD201">
         <v>1000</v>
@@ -8042,7 +8042,7 @@
         <v>3.8821697235107367E-4</v>
       </c>
       <c r="S231" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="T231">
         <v>1001</v>
@@ -8058,7 +8058,7 @@
         <v>231</v>
       </c>
       <c r="AB231" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AD231">
         <v>1000</v>
@@ -8086,7 +8086,7 @@
         <v>749</v>
       </c>
       <c r="S232" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="T232">
         <v>1001</v>
@@ -8318,7 +8318,7 @@
         <v>3.8821697235107367E-4</v>
       </c>
       <c r="S241" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="U241">
         <v>10</v>
@@ -8356,7 +8356,7 @@
         <v>55</v>
       </c>
       <c r="S242" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="V242" s="3"/>
       <c r="X242" s="1" t="s">
@@ -8382,7 +8382,7 @@
         <v>81</v>
       </c>
       <c r="S243" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="V243" s="3"/>
       <c r="X243" s="1" t="s">
@@ -8408,7 +8408,7 @@
         <v>107</v>
       </c>
       <c r="S244" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="V244" s="3"/>
       <c r="X244" s="1" t="s">
@@ -8434,7 +8434,7 @@
         <v>133</v>
       </c>
       <c r="S245" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="V245" s="3"/>
       <c r="X245" s="1" t="s">
@@ -8460,7 +8460,7 @@
         <v>162</v>
       </c>
       <c r="S246" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="V246" s="3"/>
       <c r="X246" s="1" t="s">
@@ -8486,7 +8486,7 @@
         <v>175</v>
       </c>
       <c r="S247" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="V247" s="3"/>
       <c r="X247" s="1" t="s">
@@ -8512,7 +8512,7 @@
         <v>213</v>
       </c>
       <c r="S248" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="V248" s="3"/>
       <c r="X248" s="1" t="s">
@@ -8538,7 +8538,7 @@
         <v>244</v>
       </c>
       <c r="S249" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="V249" s="3"/>
       <c r="X249" s="1" t="s">
@@ -8564,7 +8564,7 @@
         <v>272</v>
       </c>
       <c r="S250" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="V250" s="3"/>
       <c r="X250" s="1" t="s">
@@ -8603,7 +8603,7 @@
         <v>3.8821697235107367E-4</v>
       </c>
       <c r="S251" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="U251">
         <v>100</v>
@@ -8641,7 +8641,7 @@
         <v>484</v>
       </c>
       <c r="S252" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="V252" s="3"/>
       <c r="X252" s="1" t="s">
@@ -8667,7 +8667,7 @@
         <v>673</v>
       </c>
       <c r="S253" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="V253" s="3"/>
       <c r="X253" s="1" t="s">
@@ -8693,7 +8693,7 @@
         <v>928</v>
       </c>
       <c r="S254" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="V254" s="3"/>
       <c r="X254" s="1" t="s">
@@ -8870,7 +8870,7 @@
         <v>3.8821697235107367E-4</v>
       </c>
       <c r="S261" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="U261">
         <v>1000</v>
@@ -8883,7 +8883,7 @@
         <v>261</v>
       </c>
       <c r="AB261" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AD261">
         <v>1000</v>

</xml_diff>